<commit_message>
added terms,states and events for certificates
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="934">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2630,7 +2630,7 @@
     <t xml:space="preserve">Nominal Price</t>
   </si>
   <si>
-    <t xml:space="preserve">NP</t>
+    <t xml:space="preserve">NPR</t>
   </si>
   <si>
     <t xml:space="preserve">issuePrice</t>
@@ -2642,72 +2642,93 @@
     <t xml:space="preserve">IPR</t>
   </si>
   <si>
-    <t xml:space="preserve">minimumSubscription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum Subscription</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MSU</t>
+    <t xml:space="preserve">ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycleAnchorDateOfRedemption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycle Anchor Date Of Redemption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDANX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycleOfRedemption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycle Of Redemption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycleAnchorDateOfTermination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycle Anchor Date Of Termination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDANX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycleOfTermination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycle Of Termination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exercisePeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The period within which an option holder (e.g. from redemption of a note / certificate / etc) can chose to execute his option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exerciseQuantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XQ</t>
   </si>
   <si>
     <t xml:space="preserve">Integer</t>
   </si>
   <si>
-    <t xml:space="preserve">ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cycleAnchorDateOfRedemption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cycle Anchor Date Of Redemption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RDANX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cycleOfRedemption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cycle Of Redemption</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RDCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exercisePeriod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exercise Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The period within which an option holder (e.g. from redemption of a note / certificate / etc) can chose to execute his option</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exerciseQuantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exercise Quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XQ</t>
-  </si>
-  <si>
     <t xml:space="preserve">The number of shares / notes / certificates / etc executed. E.g. the number of certificates redeemed as per a certain redemption day.</t>
   </si>
   <si>
+    <t xml:space="preserve">exerciseQuantityOrdered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise Quantity Ordered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of shares / notes / certificates / etc ordered for exercise. E.g. the number of certificates ordered for redemption as per a certain redemption day.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute Applicability Rules</t>
   </si>
   <si>
@@ -2952,9 +2973,6 @@
   </si>
   <si>
     <t xml:space="preserve">The multiplier being applied to interest cash flows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPR</t>
   </si>
   <si>
     <t xml:space="preserve">The value at which principal is being repaid. This may be including or excluding of interest depending on the Contract Type</t>
@@ -3028,9 +3046,10 @@
 option: 17, identifier: scalingIndexFixing, name: Scaling Index Fixing, acronym: SC, description: Scheduled fixing of a scaling index, sequence: 17
 option: 18, identifier: interestCalculationBaseFixing, name: Interest Calculation Base Fixing, acronym: IPCB, description: Scheduled fixing of the interest calculation base, sequence: 18
 option: 19, identifier: maturity, name: Maturity, acronym: MD, description: Maturity of a contract, sequence: 19
-Option: 20, identifier: redemptionDay, name: Redemption Day, acronym: RD, description: Fixing of the redemption amount, sequence: 20
-option: 21, identifier: exercise, name: Exercise, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 21
-Option: 22, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 22</t>
+option: 20, identifier: redemptionDay, name: Redemption Day, acronym: RD, description: Fixing of the redemption amount, sequence: 20
+option: 21, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 21
+option: 22, identifier: exercise, name: Exercise, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 22
+option: 23, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 23</t>
   </si>
   <si>
     <t xml:space="preserve">The currency in which the event payoff is scheduled</t>
@@ -3481,8 +3500,8 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5405,12 +5424,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AC124"/>
+  <dimension ref="A1:AF126"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12162,11 +12181,11 @@
         <v>784</v>
       </c>
       <c r="E119" s="19" t="s">
-        <v>785</v>
+        <v>306</v>
       </c>
       <c r="F119" s="19"/>
-      <c r="G119" s="19" t="n">
-        <v>1</v>
+      <c r="G119" s="19" t="s">
+        <v>11</v>
       </c>
       <c r="H119" s="19"/>
       <c r="I119" s="19"/>
@@ -12177,24 +12196,22 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="19" t="s">
+        <v>785</v>
+      </c>
+      <c r="B120" s="19" t="s">
+        <v>616</v>
+      </c>
+      <c r="C120" s="19" t="s">
         <v>786</v>
       </c>
-      <c r="B120" s="19" t="s">
-        <v>479</v>
-      </c>
-      <c r="C120" s="19" t="s">
+      <c r="D120" s="19" t="s">
         <v>787</v>
       </c>
-      <c r="D120" s="19" t="s">
-        <v>788</v>
-      </c>
       <c r="E120" s="19" t="s">
-        <v>306</v>
+        <v>237</v>
       </c>
       <c r="F120" s="19"/>
-      <c r="G120" s="19" t="s">
-        <v>11</v>
-      </c>
+      <c r="G120" s="19"/>
       <c r="H120" s="19"/>
       <c r="I120" s="19"/>
       <c r="AB120" s="0" t="s">
@@ -12204,21 +12221,23 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="19" t="s">
+        <v>788</v>
+      </c>
+      <c r="B121" s="19" t="s">
+        <v>616</v>
+      </c>
+      <c r="C121" s="19" t="s">
         <v>789</v>
       </c>
-      <c r="B121" s="19" t="s">
-        <v>479</v>
-      </c>
-      <c r="C121" s="19" t="s">
+      <c r="D121" s="19" t="s">
         <v>790</v>
       </c>
-      <c r="D121" s="19" t="s">
-        <v>791</v>
-      </c>
       <c r="E121" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="F121" s="19"/>
+        <v>335</v>
+      </c>
+      <c r="F121" s="19" t="s">
+        <v>336</v>
+      </c>
       <c r="G121" s="19"/>
       <c r="H121" s="19"/>
       <c r="I121" s="19"/>
@@ -12229,23 +12248,21 @@
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="19" t="s">
+        <v>791</v>
+      </c>
+      <c r="B122" s="19" t="s">
+        <v>616</v>
+      </c>
+      <c r="C122" s="19" t="s">
         <v>792</v>
       </c>
-      <c r="B122" s="19" t="s">
-        <v>479</v>
-      </c>
-      <c r="C122" s="19" t="s">
+      <c r="D122" s="19" t="s">
         <v>793</v>
       </c>
-      <c r="D122" s="19" t="s">
-        <v>794</v>
-      </c>
       <c r="E122" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="F122" s="19" t="s">
-        <v>336</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="F122" s="19"/>
       <c r="G122" s="19"/>
       <c r="H122" s="19"/>
       <c r="I122" s="19"/>
@@ -12254,62 +12271,161 @@
       </c>
       <c r="AC122" s="19"/>
     </row>
-    <row r="123" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="19" t="s">
+        <v>794</v>
+      </c>
+      <c r="B123" s="19" t="s">
+        <v>616</v>
+      </c>
+      <c r="C123" s="19" t="s">
         <v>795</v>
       </c>
-      <c r="B123" s="19" t="s">
-        <v>744</v>
-      </c>
-      <c r="C123" s="19" t="s">
+      <c r="D123" s="19" t="s">
         <v>796</v>
       </c>
-      <c r="D123" s="19" t="s">
-        <v>797</v>
-      </c>
       <c r="E123" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="F123" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="G123" s="19" t="s">
-        <v>798</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="F123" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="G123" s="19"/>
       <c r="H123" s="19"/>
-      <c r="I123" s="19" t="s">
-        <v>799</v>
-      </c>
+      <c r="I123" s="19"/>
       <c r="AB123" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC123" s="19"/>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+    <row r="124" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="19" t="s">
+        <v>797</v>
+      </c>
+      <c r="B124" s="19" t="s">
+        <v>744</v>
+      </c>
+      <c r="C124" s="19" t="s">
+        <v>798</v>
+      </c>
+      <c r="D124" s="19" t="s">
+        <v>799</v>
+      </c>
+      <c r="E124" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="F124" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="G124" s="19" t="s">
         <v>800</v>
       </c>
-      <c r="B124" s="0" t="s">
-        <v>744</v>
-      </c>
-      <c r="C124" s="0" t="s">
+      <c r="H124" s="19"/>
+      <c r="I124" s="19" t="s">
         <v>801</v>
-      </c>
-      <c r="D124" s="0" t="s">
-        <v>802</v>
-      </c>
-      <c r="E124" s="0" t="s">
-        <v>785</v>
-      </c>
-      <c r="G124" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I124" s="5" t="s">
-        <v>803</v>
       </c>
       <c r="AB124" s="0" t="s">
         <v>214</v>
       </c>
+      <c r="AC124" s="19"/>
+    </row>
+    <row r="125" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="19" t="s">
+        <v>802</v>
+      </c>
+      <c r="B125" s="19" t="s">
+        <v>744</v>
+      </c>
+      <c r="C125" s="19" t="s">
+        <v>803</v>
+      </c>
+      <c r="D125" s="19" t="s">
+        <v>804</v>
+      </c>
+      <c r="E125" s="19" t="s">
+        <v>805</v>
+      </c>
+      <c r="F125" s="19"/>
+      <c r="G125" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" s="19"/>
+      <c r="I125" s="19" t="s">
+        <v>806</v>
+      </c>
+      <c r="J125" s="19"/>
+      <c r="K125" s="19"/>
+      <c r="L125" s="19"/>
+      <c r="M125" s="19"/>
+      <c r="N125" s="19"/>
+      <c r="O125" s="19"/>
+      <c r="P125" s="19"/>
+      <c r="Q125" s="19"/>
+      <c r="R125" s="19"/>
+      <c r="S125" s="19"/>
+      <c r="T125" s="19"/>
+      <c r="U125" s="19"/>
+      <c r="V125" s="19"/>
+      <c r="W125" s="19"/>
+      <c r="X125" s="19"/>
+      <c r="Y125" s="19"/>
+      <c r="Z125" s="19"/>
+      <c r="AA125" s="19"/>
+      <c r="AB125" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC125" s="19"/>
+      <c r="AD125" s="19"/>
+      <c r="AE125" s="19"/>
+      <c r="AF125" s="19"/>
+    </row>
+    <row r="126" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="19" t="s">
+        <v>807</v>
+      </c>
+      <c r="B126" s="19" t="s">
+        <v>744</v>
+      </c>
+      <c r="C126" s="19" t="s">
+        <v>808</v>
+      </c>
+      <c r="D126" s="19" t="s">
+        <v>809</v>
+      </c>
+      <c r="E126" s="19" t="s">
+        <v>805</v>
+      </c>
+      <c r="F126" s="19"/>
+      <c r="G126" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H126" s="19"/>
+      <c r="I126" s="19" t="s">
+        <v>810</v>
+      </c>
+      <c r="J126" s="19"/>
+      <c r="K126" s="19"/>
+      <c r="L126" s="19"/>
+      <c r="M126" s="19"/>
+      <c r="N126" s="19"/>
+      <c r="O126" s="19"/>
+      <c r="P126" s="19"/>
+      <c r="Q126" s="19"/>
+      <c r="R126" s="19"/>
+      <c r="S126" s="19"/>
+      <c r="T126" s="19"/>
+      <c r="U126" s="19"/>
+      <c r="V126" s="19"/>
+      <c r="W126" s="19"/>
+      <c r="X126" s="19"/>
+      <c r="Y126" s="19"/>
+      <c r="Z126" s="19"/>
+      <c r="AA126" s="19"/>
+      <c r="AB126" s="19"/>
+      <c r="AC126" s="19"/>
+      <c r="AD126" s="19"/>
+      <c r="AE126" s="19"/>
+      <c r="AF126" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="T1:T115"/>
@@ -12378,7 +12494,7 @@
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="30" t="s">
-        <v>804</v>
+        <v>811</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -12436,7 +12552,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30"/>
       <c r="B4" s="30" t="s">
-        <v>805</v>
+        <v>812</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -12494,10 +12610,10 @@
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30"/>
       <c r="B6" s="30" t="s">
-        <v>806</v>
+        <v>813</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>807</v>
+        <v>814</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="30"/>
@@ -12527,7 +12643,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="30" t="s">
-        <v>808</v>
+        <v>815</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -12584,10 +12700,10 @@
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30"/>
       <c r="B9" s="30" t="s">
-        <v>809</v>
+        <v>816</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>810</v>
+        <v>817</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="30"/>
@@ -12617,11 +12733,11 @@
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="30" t="s">
-        <v>811</v>
+        <v>818</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="30" t="s">
-        <v>812</v>
+        <v>819</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -12676,12 +12792,12 @@
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
       <c r="B12" s="30" t="s">
-        <v>813</v>
+        <v>820</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="21" t="s">
-        <v>814</v>
+        <v>821</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -12736,14 +12852,14 @@
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="30" t="s">
-        <v>815</v>
+        <v>822</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>816</v>
+        <v>823</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="21" t="s">
-        <v>817</v>
+        <v>824</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -12800,10 +12916,10 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="30" t="s">
-        <v>818</v>
+        <v>825</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>819</v>
+        <v>826</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -12832,10 +12948,10 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="30" t="s">
-        <v>820</v>
+        <v>827</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>821</v>
+        <v>828</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -12864,10 +12980,10 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="30" t="s">
-        <v>822</v>
+        <v>829</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>823</v>
+        <v>830</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -12923,11 +13039,11 @@
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="30" t="s">
-        <v>824</v>
+        <v>831</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="21" t="s">
-        <v>825</v>
+        <v>832</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -12984,10 +13100,10 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="30" t="s">
-        <v>818</v>
+        <v>825</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>826</v>
+        <v>833</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -13016,10 +13132,10 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="30" t="s">
-        <v>827</v>
+        <v>834</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>828</v>
+        <v>835</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -13075,11 +13191,11 @@
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="30" t="s">
-        <v>829</v>
+        <v>836</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="21" t="s">
-        <v>830</v>
+        <v>837</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -13136,10 +13252,10 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="31" t="s">
-        <v>831</v>
+        <v>838</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>832</v>
+        <v>839</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -13168,10 +13284,10 @@
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="31" t="s">
-        <v>833</v>
+        <v>840</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>834</v>
+        <v>841</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -13200,10 +13316,10 @@
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="31" t="s">
-        <v>835</v>
+        <v>842</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>836</v>
+        <v>843</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -13232,10 +13348,10 @@
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="31" t="s">
-        <v>837</v>
+        <v>844</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>838</v>
+        <v>845</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -13264,10 +13380,10 @@
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="31" t="s">
-        <v>839</v>
+        <v>846</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>840</v>
+        <v>847</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -13323,11 +13439,11 @@
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="30" t="s">
-        <v>841</v>
+        <v>848</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="21" t="s">
-        <v>842</v>
+        <v>849</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -13384,10 +13500,10 @@
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="30" t="s">
-        <v>818</v>
+        <v>825</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>843</v>
+        <v>850</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -13416,10 +13532,10 @@
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="30" t="s">
-        <v>844</v>
+        <v>851</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>845</v>
+        <v>852</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -13448,10 +13564,10 @@
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="30" t="s">
-        <v>846</v>
+        <v>853</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>847</v>
+        <v>854</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -13480,10 +13596,10 @@
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="30" t="s">
-        <v>848</v>
+        <v>855</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>849</v>
+        <v>856</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -13512,10 +13628,10 @@
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="30" t="s">
-        <v>850</v>
+        <v>857</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>851</v>
+        <v>858</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -13571,11 +13687,11 @@
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>852</v>
+        <v>859</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="21" t="s">
-        <v>853</v>
+        <v>860</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -13632,10 +13748,10 @@
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="30" t="s">
-        <v>818</v>
+        <v>825</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>854</v>
+        <v>861</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -13664,10 +13780,10 @@
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="31" t="s">
-        <v>855</v>
+        <v>862</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>856</v>
+        <v>863</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -13696,10 +13812,10 @@
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="30" t="s">
-        <v>857</v>
+        <v>864</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>858</v>
+        <v>865</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -13754,14 +13870,14 @@
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="30"/>
       <c r="B47" s="30" t="s">
-        <v>859</v>
+        <v>866</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>860</v>
+        <v>867</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="21" t="s">
-        <v>861</v>
+        <v>868</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
@@ -13791,7 +13907,7 @@
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
       <c r="E48" s="21" t="s">
-        <v>862</v>
+        <v>869</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
@@ -13821,7 +13937,7 @@
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
       <c r="E49" s="21" t="s">
-        <v>863</v>
+        <v>870</v>
       </c>
       <c r="F49" s="30"/>
       <c r="G49" s="30"/>
@@ -14812,10 +14928,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14858,7 +14974,7 @@
         <v>236</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>864</v>
+        <v>871</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>237</v>
@@ -14878,7 +14994,7 @@
         <v>273</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>865</v>
+        <v>872</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>210</v>
@@ -14898,7 +15014,7 @@
         <v>285</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>866</v>
+        <v>873</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>237</v>
@@ -14918,7 +15034,7 @@
         <v>432</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>867</v>
+        <v>874</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>306</v>
@@ -14935,7 +15051,7 @@
         <v>513</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>868</v>
+        <v>875</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>306</v>
@@ -14952,7 +15068,7 @@
         <v>400</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>306</v>
@@ -14969,7 +15085,7 @@
         <v>404</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>869</v>
+        <v>876</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>306</v>
@@ -14986,7 +15102,7 @@
         <v>413</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>870</v>
+        <v>877</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>306</v>
@@ -14994,16 +15110,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>871</v>
+        <v>878</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>872</v>
+        <v>879</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>873</v>
+        <v>880</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>874</v>
+        <v>881</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>306</v>
@@ -15020,7 +15136,7 @@
         <v>373</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>875</v>
+        <v>882</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>306</v>
@@ -15034,10 +15150,10 @@
         <v>436</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>876</v>
+        <v>883</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>877</v>
+        <v>884</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>306</v>
@@ -15045,16 +15161,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>878</v>
+        <v>885</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>879</v>
+        <v>886</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>880</v>
+        <v>887</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>881</v>
+        <v>888</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>306</v>
@@ -15062,16 +15178,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>882</v>
+        <v>889</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>883</v>
+        <v>890</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>884</v>
+        <v>891</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>885</v>
+        <v>892</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>306</v>
@@ -15085,10 +15201,10 @@
         <v>547</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>886</v>
+        <v>778</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>887</v>
+        <v>893</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>306</v>
@@ -15105,7 +15221,7 @@
         <v>746</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>888</v>
+        <v>894</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>237</v>
@@ -15125,7 +15241,7 @@
         <v>751</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>889</v>
+        <v>895</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>306</v>
@@ -15133,58 +15249,75 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>803</v>
+        <v>806</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>890</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="D20" s="5" t="s">
+        <v>896</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F20" s="0" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B21" s="0" t="s">
         <v>506</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>891</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="D21" s="0" t="s">
+        <v>897</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F21" s="0" t="s">
         <v>238</v>
       </c>
     </row>
@@ -15242,16 +15375,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>892</v>
+        <v>898</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>893</v>
+        <v>899</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>894</v>
+        <v>900</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>895</v>
+        <v>901</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -15262,16 +15395,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>896</v>
+        <v>902</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>897</v>
+        <v>903</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>898</v>
+        <v>904</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>899</v>
+        <v>905</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -15282,22 +15415,22 @@
     </row>
     <row r="4" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>900</v>
+        <v>906</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>901</v>
+        <v>907</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>902</v>
+        <v>908</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>903</v>
+        <v>909</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>904</v>
+        <v>910</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15311,7 +15444,7 @@
         <v>481</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>905</v>
+        <v>911</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -15322,16 +15455,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>906</v>
+        <v>912</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>907</v>
+        <v>913</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>908</v>
+        <v>914</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>909</v>
+        <v>915</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -15339,19 +15472,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>910</v>
+        <v>916</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>911</v>
+        <v>917</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>912</v>
+        <v>918</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>913</v>
+        <v>919</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>911</v>
+        <v>917</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15435,16 +15568,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>914</v>
+        <v>920</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>915</v>
+        <v>921</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>916</v>
+        <v>922</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>917</v>
+        <v>923</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -15452,42 +15585,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>918</v>
+        <v>924</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>919</v>
+        <v>925</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>920</v>
+        <v>926</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>921</v>
+        <v>927</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>922</v>
+        <v>928</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>923</v>
+        <v>929</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>924</v>
+        <v>930</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>925</v>
+        <v>931</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>926</v>
+        <v>932</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>927</v>
+        <v>933</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
sketched draft Certificates specifications
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="948">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2633,6 +2633,9 @@
     <t xml:space="preserve">NPR</t>
   </si>
   <si>
+    <t xml:space="preserve">The nominal price for a single certificate.</t>
+  </si>
+  <si>
     <t xml:space="preserve">issuePrice</t>
   </si>
   <si>
@@ -2642,33 +2645,45 @@
     <t xml:space="preserve">IPR</t>
   </si>
   <si>
-    <t xml:space="preserve">ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio</t>
+    <t xml:space="preserve">The issue price for a single certificate as per Issue Day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denominationRatio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denomination Ratio</t>
   </si>
   <si>
     <t xml:space="preserve">RAT</t>
   </si>
   <si>
+    <t xml:space="preserve">The ratio defining how a single certificate is denominated in terms of the certificate’s underlying instrument. Is often times also simply referred to as the “Ratio”.</t>
+  </si>
+  <si>
     <t xml:space="preserve">cycleAnchorDateOfRedemption</t>
   </si>
   <si>
-    <t xml:space="preserve">Cycle Anchor Date Of Redemption</t>
+    <t xml:space="preserve">Cycle Anchor Date Of Redemption Day</t>
   </si>
   <si>
     <t xml:space="preserve">RDANX</t>
   </si>
   <si>
+    <t xml:space="preserve">The start date of the Redemption Day schedule. i.e. this is the very first regular Redemption Day. After this day periodic Redemption Days are scheduled through the Cycle of Redemption Day.</t>
+  </si>
+  <si>
     <t xml:space="preserve">cycleOfRedemption</t>
   </si>
   <si>
-    <t xml:space="preserve">Cycle Of Redemption</t>
+    <t xml:space="preserve">Cycle Of Redemption Day</t>
   </si>
   <si>
     <t xml:space="preserve">RDCL</t>
   </si>
   <si>
+    <t xml:space="preserve">The period according to which Redemption Days are scheduled.</t>
+  </si>
+  <si>
     <t xml:space="preserve">cycleAnchorDateOfTermination</t>
   </si>
   <si>
@@ -2678,6 +2693,9 @@
     <t xml:space="preserve">TDANX</t>
   </si>
   <si>
+    <t xml:space="preserve">The start date of the Termination Day schedule. i.e. this is the very first regular Termination Day. After this period Termination Days are scheduled according to the Cycle Of Termination Day.</t>
+  </si>
+  <si>
     <t xml:space="preserve">cycleOfTermination</t>
   </si>
   <si>
@@ -2687,6 +2705,9 @@
     <t xml:space="preserve">TDCL</t>
   </si>
   <si>
+    <t xml:space="preserve">The period according to which Termination Days are scheduled.</t>
+  </si>
+  <si>
     <t xml:space="preserve">exercisePeriod</t>
   </si>
   <si>
@@ -2727,6 +2748,27 @@
   </si>
   <si>
     <t xml:space="preserve">The number of shares / notes / certificates / etc ordered for exercise. E.g. the number of certificates ordered for redemption as per a certain redemption day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marginFactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Margin Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A correction factor for the Redemption Amount determined by the Calculating Agent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjustmentFactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjustment Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADF</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute Applicability Rules</t>
@@ -5424,12 +5466,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AF126"/>
+  <dimension ref="A1:AF128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8914,7 +8956,9 @@
       <c r="Y57" s="22"/>
       <c r="Z57" s="22"/>
       <c r="AA57" s="22"/>
-      <c r="AB57" s="22"/>
+      <c r="AB57" s="22" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="19" t="s">
@@ -9037,7 +9081,7 @@
       </c>
       <c r="AA59" s="22"/>
       <c r="AB59" s="22" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11852,7 +11896,9 @@
         <v>753</v>
       </c>
       <c r="AA111" s="19"/>
-      <c r="AB111" s="19"/>
+      <c r="AB111" s="19" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="19" t="s">
@@ -12136,7 +12182,9 @@
       <c r="F117" s="19"/>
       <c r="G117" s="19"/>
       <c r="H117" s="19"/>
-      <c r="I117" s="19"/>
+      <c r="I117" s="19" t="s">
+        <v>779</v>
+      </c>
       <c r="AB117" s="0" t="s">
         <v>233</v>
       </c>
@@ -12144,16 +12192,16 @@
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="19" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B118" s="19" t="s">
         <v>479</v>
       </c>
       <c r="C118" s="19" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="D118" s="19" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="E118" s="19" t="s">
         <v>306</v>
@@ -12161,24 +12209,26 @@
       <c r="F118" s="19"/>
       <c r="G118" s="19"/>
       <c r="H118" s="19"/>
-      <c r="I118" s="19"/>
+      <c r="I118" s="19" t="s">
+        <v>783</v>
+      </c>
       <c r="AB118" s="0" t="s">
         <v>233</v>
       </c>
       <c r="AC118" s="19"/>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="19" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="B119" s="19" t="s">
         <v>479</v>
       </c>
       <c r="C119" s="19" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D119" s="19" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="E119" s="19" t="s">
         <v>306</v>
@@ -12188,24 +12238,26 @@
         <v>11</v>
       </c>
       <c r="H119" s="19"/>
-      <c r="I119" s="19"/>
+      <c r="I119" s="19" t="s">
+        <v>787</v>
+      </c>
       <c r="AB119" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC119" s="19"/>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="19" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="B120" s="19" t="s">
         <v>616</v>
       </c>
       <c r="C120" s="19" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="D120" s="19" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="E120" s="19" t="s">
         <v>237</v>
@@ -12213,7 +12265,9 @@
       <c r="F120" s="19"/>
       <c r="G120" s="19"/>
       <c r="H120" s="19"/>
-      <c r="I120" s="19"/>
+      <c r="I120" s="19" t="s">
+        <v>791</v>
+      </c>
       <c r="AB120" s="0" t="s">
         <v>214</v>
       </c>
@@ -12221,16 +12275,16 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="19" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
       <c r="B121" s="19" t="s">
         <v>616</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
       <c r="D121" s="19" t="s">
-        <v>790</v>
+        <v>794</v>
       </c>
       <c r="E121" s="19" t="s">
         <v>335</v>
@@ -12240,24 +12294,26 @@
       </c>
       <c r="G121" s="19"/>
       <c r="H121" s="19"/>
-      <c r="I121" s="19"/>
+      <c r="I121" s="19" t="s">
+        <v>795</v>
+      </c>
       <c r="AB121" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC121" s="19"/>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="19" t="s">
-        <v>791</v>
+        <v>796</v>
       </c>
       <c r="B122" s="19" t="s">
         <v>616</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>792</v>
+        <v>797</v>
       </c>
       <c r="D122" s="19" t="s">
-        <v>793</v>
+        <v>798</v>
       </c>
       <c r="E122" s="19" t="s">
         <v>237</v>
@@ -12265,7 +12321,9 @@
       <c r="F122" s="19"/>
       <c r="G122" s="19"/>
       <c r="H122" s="19"/>
-      <c r="I122" s="19"/>
+      <c r="I122" s="19" t="s">
+        <v>799</v>
+      </c>
       <c r="AB122" s="0" t="s">
         <v>214</v>
       </c>
@@ -12273,16 +12331,16 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="19" t="s">
-        <v>794</v>
+        <v>800</v>
       </c>
       <c r="B123" s="19" t="s">
         <v>616</v>
       </c>
       <c r="C123" s="19" t="s">
-        <v>795</v>
+        <v>801</v>
       </c>
       <c r="D123" s="19" t="s">
-        <v>796</v>
+        <v>802</v>
       </c>
       <c r="E123" s="19" t="s">
         <v>335</v>
@@ -12292,7 +12350,9 @@
       </c>
       <c r="G123" s="19"/>
       <c r="H123" s="19"/>
-      <c r="I123" s="19"/>
+      <c r="I123" s="19" t="s">
+        <v>803</v>
+      </c>
       <c r="AB123" s="0" t="s">
         <v>214</v>
       </c>
@@ -12300,16 +12360,16 @@
     </row>
     <row r="124" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="19" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="B124" s="19" t="s">
         <v>744</v>
       </c>
       <c r="C124" s="19" t="s">
-        <v>798</v>
+        <v>805</v>
       </c>
       <c r="D124" s="19" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
       <c r="E124" s="19" t="s">
         <v>290</v>
@@ -12318,11 +12378,11 @@
         <v>291</v>
       </c>
       <c r="G124" s="19" t="s">
-        <v>800</v>
+        <v>807</v>
       </c>
       <c r="H124" s="19"/>
       <c r="I124" s="19" t="s">
-        <v>801</v>
+        <v>808</v>
       </c>
       <c r="AB124" s="0" t="s">
         <v>214</v>
@@ -12331,19 +12391,19 @@
     </row>
     <row r="125" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="19" t="s">
-        <v>802</v>
+        <v>809</v>
       </c>
       <c r="B125" s="19" t="s">
         <v>744</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="D125" s="19" t="s">
-        <v>804</v>
+        <v>811</v>
       </c>
       <c r="E125" s="19" t="s">
-        <v>805</v>
+        <v>812</v>
       </c>
       <c r="F125" s="19"/>
       <c r="G125" s="19" t="n">
@@ -12351,7 +12411,7 @@
       </c>
       <c r="H125" s="19"/>
       <c r="I125" s="19" t="s">
-        <v>806</v>
+        <v>813</v>
       </c>
       <c r="J125" s="19"/>
       <c r="K125" s="19"/>
@@ -12379,21 +12439,21 @@
       <c r="AE125" s="19"/>
       <c r="AF125" s="19"/>
     </row>
-    <row r="126" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="19" t="s">
-        <v>807</v>
+        <v>814</v>
       </c>
       <c r="B126" s="19" t="s">
         <v>744</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>808</v>
+        <v>815</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>809</v>
+        <v>816</v>
       </c>
       <c r="E126" s="19" t="s">
-        <v>805</v>
+        <v>812</v>
       </c>
       <c r="F126" s="19"/>
       <c r="G126" s="19" t="n">
@@ -12401,7 +12461,7 @@
       </c>
       <c r="H126" s="19"/>
       <c r="I126" s="19" t="s">
-        <v>810</v>
+        <v>817</v>
       </c>
       <c r="J126" s="19"/>
       <c r="K126" s="19"/>
@@ -12421,11 +12481,65 @@
       <c r="Y126" s="19"/>
       <c r="Z126" s="19"/>
       <c r="AA126" s="19"/>
-      <c r="AB126" s="19"/>
+      <c r="AB126" s="19" t="s">
+        <v>214</v>
+      </c>
       <c r="AC126" s="19"/>
       <c r="AD126" s="19"/>
       <c r="AE126" s="19"/>
       <c r="AF126" s="19"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>818</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="D127" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="E127" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="G127" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I127" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="AB127" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>822</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>744</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>823</v>
+      </c>
+      <c r="D128" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="E128" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="G128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I128" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="AB128" s="0" t="s">
+        <v>214</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="T1:T115"/>
@@ -12494,7 +12608,7 @@
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="30" t="s">
-        <v>811</v>
+        <v>825</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -12552,7 +12666,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30"/>
       <c r="B4" s="30" t="s">
-        <v>812</v>
+        <v>826</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -12610,10 +12724,10 @@
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30"/>
       <c r="B6" s="30" t="s">
-        <v>813</v>
+        <v>827</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>814</v>
+        <v>828</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="30"/>
@@ -12643,7 +12757,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="30" t="s">
-        <v>815</v>
+        <v>829</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -12700,10 +12814,10 @@
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30"/>
       <c r="B9" s="30" t="s">
-        <v>816</v>
+        <v>830</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>817</v>
+        <v>831</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="30"/>
@@ -12733,11 +12847,11 @@
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="30" t="s">
-        <v>818</v>
+        <v>832</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="30" t="s">
-        <v>819</v>
+        <v>833</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -12792,12 +12906,12 @@
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
       <c r="B12" s="30" t="s">
-        <v>820</v>
+        <v>834</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="21" t="s">
-        <v>821</v>
+        <v>835</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -12852,14 +12966,14 @@
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="30" t="s">
-        <v>822</v>
+        <v>836</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>823</v>
+        <v>837</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="21" t="s">
-        <v>824</v>
+        <v>838</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -12916,10 +13030,10 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="30" t="s">
-        <v>825</v>
+        <v>839</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>826</v>
+        <v>840</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -12948,10 +13062,10 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="30" t="s">
-        <v>827</v>
+        <v>841</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>828</v>
+        <v>842</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -12980,10 +13094,10 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="30" t="s">
-        <v>829</v>
+        <v>843</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>830</v>
+        <v>844</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -13039,11 +13153,11 @@
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="30" t="s">
-        <v>831</v>
+        <v>845</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="21" t="s">
-        <v>832</v>
+        <v>846</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -13100,10 +13214,10 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="30" t="s">
-        <v>825</v>
+        <v>839</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>833</v>
+        <v>847</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -13132,10 +13246,10 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="30" t="s">
-        <v>834</v>
+        <v>848</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>835</v>
+        <v>849</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -13191,11 +13305,11 @@
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="30" t="s">
-        <v>836</v>
+        <v>850</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="21" t="s">
-        <v>837</v>
+        <v>851</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -13252,10 +13366,10 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="31" t="s">
-        <v>838</v>
+        <v>852</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>839</v>
+        <v>853</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -13284,10 +13398,10 @@
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="31" t="s">
-        <v>840</v>
+        <v>854</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>841</v>
+        <v>855</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -13316,10 +13430,10 @@
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="31" t="s">
-        <v>842</v>
+        <v>856</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>843</v>
+        <v>857</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -13348,10 +13462,10 @@
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="31" t="s">
-        <v>844</v>
+        <v>858</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>845</v>
+        <v>859</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -13380,10 +13494,10 @@
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="31" t="s">
-        <v>846</v>
+        <v>860</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>847</v>
+        <v>861</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -13439,11 +13553,11 @@
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="30" t="s">
-        <v>848</v>
+        <v>862</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="21" t="s">
-        <v>849</v>
+        <v>863</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -13500,10 +13614,10 @@
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="30" t="s">
-        <v>825</v>
+        <v>839</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>850</v>
+        <v>864</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -13532,10 +13646,10 @@
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="30" t="s">
-        <v>851</v>
+        <v>865</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>852</v>
+        <v>866</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -13564,10 +13678,10 @@
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="30" t="s">
-        <v>853</v>
+        <v>867</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>854</v>
+        <v>868</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -13596,10 +13710,10 @@
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="30" t="s">
-        <v>855</v>
+        <v>869</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>856</v>
+        <v>870</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -13628,10 +13742,10 @@
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="30" t="s">
-        <v>857</v>
+        <v>871</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>858</v>
+        <v>872</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -13687,11 +13801,11 @@
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>859</v>
+        <v>873</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="21" t="s">
-        <v>860</v>
+        <v>874</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -13748,10 +13862,10 @@
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="30" t="s">
-        <v>825</v>
+        <v>839</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>861</v>
+        <v>875</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -13780,10 +13894,10 @@
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="31" t="s">
-        <v>862</v>
+        <v>876</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>863</v>
+        <v>877</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -13812,10 +13926,10 @@
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="30" t="s">
-        <v>864</v>
+        <v>878</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>865</v>
+        <v>879</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -13870,14 +13984,14 @@
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="30"/>
       <c r="B47" s="30" t="s">
-        <v>866</v>
+        <v>880</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>867</v>
+        <v>881</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="21" t="s">
-        <v>868</v>
+        <v>882</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
@@ -13907,7 +14021,7 @@
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
       <c r="E48" s="21" t="s">
-        <v>869</v>
+        <v>883</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
@@ -13937,7 +14051,7 @@
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
       <c r="E49" s="21" t="s">
-        <v>870</v>
+        <v>884</v>
       </c>
       <c r="F49" s="30"/>
       <c r="G49" s="30"/>
@@ -14928,10 +15042,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14974,7 +15088,7 @@
         <v>236</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>871</v>
+        <v>885</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>237</v>
@@ -14994,7 +15108,7 @@
         <v>273</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>872</v>
+        <v>886</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>210</v>
@@ -15014,7 +15128,7 @@
         <v>285</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>873</v>
+        <v>887</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>237</v>
@@ -15034,7 +15148,7 @@
         <v>432</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>874</v>
+        <v>888</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>306</v>
@@ -15051,7 +15165,7 @@
         <v>513</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>875</v>
+        <v>889</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>306</v>
@@ -15068,7 +15182,7 @@
         <v>400</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>876</v>
+        <v>890</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>306</v>
@@ -15085,7 +15199,7 @@
         <v>404</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>876</v>
+        <v>890</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>306</v>
@@ -15102,7 +15216,7 @@
         <v>413</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>877</v>
+        <v>891</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>306</v>
@@ -15110,16 +15224,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>878</v>
+        <v>892</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>879</v>
+        <v>893</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>880</v>
+        <v>894</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>881</v>
+        <v>895</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>306</v>
@@ -15136,7 +15250,7 @@
         <v>373</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>882</v>
+        <v>896</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>306</v>
@@ -15150,10 +15264,10 @@
         <v>436</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>883</v>
+        <v>897</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>884</v>
+        <v>898</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>306</v>
@@ -15161,16 +15275,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>885</v>
+        <v>899</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>886</v>
+        <v>900</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>887</v>
+        <v>901</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>888</v>
+        <v>902</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>306</v>
@@ -15178,16 +15292,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>889</v>
+        <v>903</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>890</v>
+        <v>904</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>891</v>
+        <v>905</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>892</v>
+        <v>906</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>306</v>
@@ -15204,7 +15318,7 @@
         <v>778</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>893</v>
+        <v>907</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>306</v>
@@ -15221,7 +15335,7 @@
         <v>746</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>894</v>
+        <v>908</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>237</v>
@@ -15241,7 +15355,7 @@
         <v>751</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>895</v>
+        <v>909</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>306</v>
@@ -15249,75 +15363,109 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>802</v>
+        <v>809</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>804</v>
+        <v>811</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>806</v>
+        <v>813</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>805</v>
+        <v>812</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>807</v>
+        <v>814</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>808</v>
+        <v>815</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>809</v>
+        <v>816</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>810</v>
+        <v>817</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>818</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>819</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>822</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>823</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B22" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C22" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>896</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="D22" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F22" s="0" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B23" s="0" t="s">
         <v>506</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>897</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="D23" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F23" s="0" t="s">
         <v>238</v>
       </c>
     </row>
@@ -15375,16 +15523,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>898</v>
+        <v>912</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>899</v>
+        <v>913</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>900</v>
+        <v>914</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>901</v>
+        <v>915</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -15395,16 +15543,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>902</v>
+        <v>916</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>903</v>
+        <v>917</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>904</v>
+        <v>918</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>905</v>
+        <v>919</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -15415,22 +15563,22 @@
     </row>
     <row r="4" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>906</v>
+        <v>920</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>907</v>
+        <v>921</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>908</v>
+        <v>922</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>909</v>
+        <v>923</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>910</v>
+        <v>924</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15444,7 +15592,7 @@
         <v>481</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>911</v>
+        <v>925</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -15455,16 +15603,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>912</v>
+        <v>926</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>913</v>
+        <v>927</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>914</v>
+        <v>928</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>915</v>
+        <v>929</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -15472,19 +15620,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>916</v>
+        <v>930</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>917</v>
+        <v>931</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>918</v>
+        <v>932</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>919</v>
+        <v>933</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>917</v>
+        <v>931</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15568,16 +15716,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>920</v>
+        <v>934</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>921</v>
+        <v>935</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>922</v>
+        <v>936</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>923</v>
+        <v>937</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -15585,42 +15733,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>924</v>
+        <v>938</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>925</v>
+        <v>939</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>926</v>
+        <v>940</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>927</v>
+        <v>941</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>928</v>
+        <v>942</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>929</v>
+        <v>943</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>930</v>
+        <v>944</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>931</v>
+        <v>945</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>932</v>
+        <v>946</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>933</v>
+        <v>947</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added ID (Issue Day) event option
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -3068,30 +3068,31 @@
     <t xml:space="preserve">The type of the event. Different types have their own business logic in terms of payoff and state transition functions</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 22
-option: 1, identifier: initialExchange, name: Initial Exchange, acronym: IED, description: Scheduled date of initial exchange of e.g. principal value in fixed income products, sequence: 1
-Option: 2, identifier: feePayment, name: Fee Payment, acronym: FP, description: Scheduled fee payments, sequence: 2
-option: 3, identifier: principalRedemption, name: Principal Redemption, acronym: PR, description: Scheduled principal redemption payment, sequence: 3
-option: 4, identifier: principalDrawing, name: Principal Drawing, acronym: PD, description: Drawing of principal amount e.g. in a credit line, sequence: 4
-option: 5, identifier: principalPaymentAmountFixing, name: Principal Payment Amount Fixing, acronym: PRF, description: Scheduled fixing of principal payment amount, sequence: 5
-option: 6, identifier: penalytPayment, name: Penalty Payment, acronym: PY, description: Scheduled payment of a penalty, sequence: 6
-option: 7, identifier: principalPrepayment, name: Principal Prepayment, acronym: PP, description: Unscheduled early repayment of principal, sequence: 7
-option: 8, identifier: interestPayment, name: Interest Payment, acronym: IP, description: Scheduled interest payment, sequence: 8
-option: 9, identifier: interestCapitalization, name: Interest Capitalization, acronym: IPCI, description: Scheduled capitalization of accrued interest, sequence: 9
-option: 10, identifier: creditEvent, name: Credit Event, acronym: CE, description: Credit event of counterparty to a contract, sequence: 10
-option: 11, identifier: rateResetFixed, name: Rate Reset Fixing with Known Rate, acronym: RRF, description: Scheduled fixing of variable rate with known new rate, sequence: 11 
-option: 12, identifier: rateResetVariable, name: Rate Reset Fixing with Unknown Rate, acronym: RR, description: Scheduled fixing of variable rate with unknown new rate, sequence: 12
-option: 13, identifier: dividendPayment, name: Dividend Payment, acronym: DV, description: Payment of dividends, sequence: 13
-option: 14, identifier: purchase, name: Purchase, acronym: PRD, description: Purchase of a contract, sequence: 14
-option: 15, identifier: marginCall, name: Margin Call, acronym: MR, description: Scheduled margin call, sequence: 15
-option: 16, identifier: termination, name: Termination, acronym: TD, description: Termination of a contract, sequence: 16
-option: 17, identifier: scalingIndexFixing, name: Scaling Index Fixing, acronym: SC, description: Scheduled fixing of a scaling index, sequence: 17
-option: 18, identifier: interestCalculationBaseFixing, name: Interest Calculation Base Fixing, acronym: IPCB, description: Scheduled fixing of the interest calculation base, sequence: 18
-option: 19, identifier: maturity, name: Maturity, acronym: MD, description: Maturity of a contract, sequence: 19
-option: 20, identifier: redemptionDay, name: Redemption Day, acronym: RD, description: Fixing of the redemption amount, sequence: 20
-option: 21, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 21
-option: 22, identifier: exercise, name: Exercise, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 22
-option: 23, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 23</t>
+    <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 25
+option: 1, identifier: issueDay, name: Issue Day, acronym: ID, description: Marks the day or timestamp respectively of issuance of a contract, sequence: 1
+option: 2, identifier: initialExchange, name: Initial Exchange, acronym: IED, description: Scheduled date of initial exchange of e.g. principal value in fixed income products, sequence: 2
+option: 3, identifier: feePayment, name: Fee Payment, acronym: FP, description: Scheduled fee payments, sequence: 3
+option: 4, identifier: principalRedemption, name: Principal Redemption, acronym: PR, description: Scheduled principal redemption payment, sequence: 4
+option: 5, identifier: principalDrawing, name: Principal Drawing, acronym: PD, description: Drawing of principal amount e.g. in a credit line, sequence: 5
+option: 6, identifier: principalPaymentAmountFixing, name: Principal Payment Amount Fixing, acronym: PRF, description: Scheduled fixing of principal payment amount, sequence: 6
+option: 7, identifier: penalytPayment, name: Penalty Payment, acronym: PY, description: Scheduled payment of a penalty, sequence: 7
+option: 8, identifier: principalPrepayment, name: Principal Prepayment, acronym: PP, description: Unscheduled early repayment of principal, sequence: 8
+option: 9, identifier: interestPayment, name: Interest Payment, acronym: IP, description: Scheduled interest payment, sequence: 9
+option: 10, identifier: interestCapitalization, name: Interest Capitalization, acronym: IPCI, description: Scheduled capitalization of accrued interest, sequence: 10
+option: 11, identifier: creditEvent, name: Credit Event, acronym: CE, description: Credit event of counterparty to a contract, sequence: 11
+option: 12, identifier: rateResetFixed, name: Rate Reset Fixing with Known Rate, acronym: RRF, description: Scheduled fixing of variable rate with known new rate, sequence: 12
+option: 13, identifier: rateResetVariable, name: Rate Reset Fixing with Unknown Rate, acronym: RR, description: Scheduled fixing of variable rate with unknown new rate, sequence: 13
+option: 14, identifier: dividendPayment, name: Dividend Payment, acronym: DV, description: Payment of dividends, sequence: 14
+option: 15, identifier: purchase, name: Purchase, acronym: PRD, description: Purchase of a contract, sequence: 15
+option: 16, identifier: marginCall, name: Margin Call, acronym: MR, description: Scheduled margin call, sequence: 16
+option: 17, identifier: termination, name: Termination, acronym: TD, description: Termination of a contract, sequence: 17
+option: 18, identifier: scalingIndexFixing, name: Scaling Index Fixing, acronym: SC, description: Scheduled fixing of a scaling index, sequence: 18
+option: 19, identifier: interestCalculationBaseFixing, name: Interest Calculation Base Fixing, acronym: IPCB, description: Scheduled fixing of the interest calculation base, sequence: 19
+option: 20, identifier: maturity, name: Maturity, acronym: MD, description: Maturity of a contract, sequence: 20
+option: 21, identifier: redemptionDay, name: Redemption Day, acronym: RD, description: Fixing of the redemption amount, sequence: 21
+option: 22, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 22
+option: 23, identifier: exercise, name: Exercise, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 23
+Option: 24, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 24</t>
   </si>
   <si>
     <t xml:space="preserve">The currency in which the event payoff is scheduled</t>
@@ -3542,8 +3543,8 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5468,7 +5469,7 @@
   </sheetPr>
   <dimension ref="A1:AF128"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A127" activeCellId="0" sqref="A127"/>

</xml_diff>

<commit_message>
Fixed dividend -> coupon schedule feature
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="971">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2771,6 +2771,79 @@
     <t xml:space="preserve">ADF</t>
   </si>
   <si>
+    <t xml:space="preserve">cycleAnchorDateOfCoupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycle Anchor Date Of Coupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPANX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The start date of the Coupon Day schedule. i.e. this is the very first regular Coupon Day. After this day periodic Coupon Days are scheduled through the Cycle of Coupon Day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycleOfCoupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycle Of Coupon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The period according to which Coupon Days are scheduled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couponType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupon Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">option: 0, identifier: none, name: No Coupon, acronym: NOC, description: No coupon is paid.
+option: 1, identifier: fixed, name: Fixed Coupon, acronym: FIX, description: A fixed coupon is paid according to the couponRate.
+option: 2, identifier: fixedConditional, name: Fixed Conditional Coupon, acronym: FCN, description: A fixed coupon is paid conditional to sufficient liquidity.
+option: 3, identifier: performance, name: Performance Based, acronym: PRF, description: The coupon paid is based on the performance of the underlying instrument.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of coupon applicable. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">couponRate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupon Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPRT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The fixed coupon applicable (if any). Applies in conjunction with couponType=FIX (fixed).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">couponAmountFixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coupon Amount Fixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPFX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The coupon amount fixed at the most recent coupon day and due for payment.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute Applicability Rules</t>
   </si>
   <si>
@@ -3068,7 +3141,7 @@
     <t xml:space="preserve">The type of the event. Different types have their own business logic in terms of payoff and state transition functions</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 25
+    <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 27
 option: 1, identifier: issueDay, name: Issue Day, acronym: ID, description: Marks the day or timestamp respectively of issuance of a contract, sequence: 1
 option: 2, identifier: initialExchange, name: Initial Exchange, acronym: IED, description: Scheduled date of initial exchange of e.g. principal value in fixed income products, sequence: 2
 option: 3, identifier: feePayment, name: Fee Payment, acronym: FP, description: Scheduled fee payments, sequence: 3
@@ -3089,10 +3162,12 @@
 option: 18, identifier: scalingIndexFixing, name: Scaling Index Fixing, acronym: SC, description: Scheduled fixing of a scaling index, sequence: 18
 option: 19, identifier: interestCalculationBaseFixing, name: Interest Calculation Base Fixing, acronym: IPCB, description: Scheduled fixing of the interest calculation base, sequence: 19
 option: 20, identifier: maturity, name: Maturity, acronym: MD, description: Maturity of a contract, sequence: 20
-option: 21, identifier: redemptionDay, name: Redemption Day, acronym: RD, description: Fixing of the redemption amount, sequence: 21
-option: 22, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 22
-option: 23, identifier: exercise, name: Exercise, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 23
-Option: 24, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 24</t>
+option: 21, identifier: couponFixingDay, name: Coupon Fixing Day, acronym: CFD, description: Fixing of the coupon amount, sequence: 21 
+option: 22, identifier: couponPaymentDay, name: Coupon Payment Day, acronym: CPD, description: Payment of the coupon amount, sequence: 22
+option: 23, identifier: redemptionDay, name: Redemption Day, acronym: RD, description: Fixing of the redemption amount, sequence: 23
+option: 24, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 24
+option: 25, identifier: exerciseDay, name: Exercise Day, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 25
+Option: 26, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 26</t>
   </si>
   <si>
     <t xml:space="preserve">The currency in which the event payoff is scheduled</t>
@@ -3544,7 +3619,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5467,12 +5542,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AF128"/>
+  <dimension ref="A1:AF133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7125,9 +7200,7 @@
       <c r="Y23" s="22"/>
       <c r="Z23" s="22"/>
       <c r="AA23" s="22"/>
-      <c r="AB23" s="19" t="s">
-        <v>331</v>
-      </c>
+      <c r="AB23" s="19"/>
     </row>
     <row r="24" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="19" t="s">
@@ -7173,9 +7246,7 @@
       <c r="Y24" s="22"/>
       <c r="Z24" s="22"/>
       <c r="AA24" s="22"/>
-      <c r="AB24" s="19" t="s">
-        <v>338</v>
-      </c>
+      <c r="AB24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
@@ -7225,9 +7296,7 @@
       <c r="Y25" s="22"/>
       <c r="Z25" s="22"/>
       <c r="AA25" s="22"/>
-      <c r="AB25" s="19" t="s">
-        <v>344</v>
-      </c>
+      <c r="AB25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
@@ -7273,9 +7342,7 @@
       <c r="Y26" s="22"/>
       <c r="Z26" s="22"/>
       <c r="AA26" s="22"/>
-      <c r="AB26" s="19" t="s">
-        <v>349</v>
-      </c>
+      <c r="AB26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
@@ -12247,7 +12314,7 @@
       </c>
       <c r="AC119" s="19"/>
     </row>
-    <row r="120" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="19" t="s">
         <v>788</v>
       </c>
@@ -12263,7 +12330,9 @@
       <c r="E120" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="F120" s="19"/>
+      <c r="F120" s="21" t="s">
+        <v>238</v>
+      </c>
       <c r="G120" s="19"/>
       <c r="H120" s="19"/>
       <c r="I120" s="19" t="s">
@@ -12303,7 +12372,7 @@
       </c>
       <c r="AC121" s="19"/>
     </row>
-    <row r="122" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="19" t="s">
         <v>796</v>
       </c>
@@ -12319,7 +12388,9 @@
       <c r="E122" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="F122" s="19"/>
+      <c r="F122" s="21" t="s">
+        <v>238</v>
+      </c>
       <c r="G122" s="19"/>
       <c r="H122" s="19"/>
       <c r="I122" s="19" t="s">
@@ -12540,6 +12611,139 @@
       </c>
       <c r="AB128" s="0" t="s">
         <v>214</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>828</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="F129" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="I129" s="19" t="s">
+        <v>829</v>
+      </c>
+      <c r="AB129" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>830</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>832</v>
+      </c>
+      <c r="E130" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="F130" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="I130" s="19" t="s">
+        <v>833</v>
+      </c>
+      <c r="AB130" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>835</v>
+      </c>
+      <c r="D131" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="E131" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="F131" s="19" t="s">
+        <v>837</v>
+      </c>
+      <c r="G131" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="I131" s="0" t="s">
+        <v>839</v>
+      </c>
+      <c r="AB131" s="19" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>841</v>
+      </c>
+      <c r="D132" s="0" t="s">
+        <v>842</v>
+      </c>
+      <c r="E132" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="G132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" s="0" t="s">
+        <v>843</v>
+      </c>
+      <c r="AB132" s="19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="D133" s="0" t="s">
+        <v>846</v>
+      </c>
+      <c r="E133" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="G133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" s="0" t="s">
+        <v>847</v>
+      </c>
+      <c r="AB133" s="19" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -12609,7 +12813,7 @@
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="30" t="s">
-        <v>825</v>
+        <v>848</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -12667,7 +12871,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30"/>
       <c r="B4" s="30" t="s">
-        <v>826</v>
+        <v>849</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -12725,10 +12929,10 @@
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30"/>
       <c r="B6" s="30" t="s">
-        <v>827</v>
+        <v>850</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>828</v>
+        <v>851</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="30"/>
@@ -12758,7 +12962,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="30" t="s">
-        <v>829</v>
+        <v>852</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -12815,10 +13019,10 @@
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30"/>
       <c r="B9" s="30" t="s">
-        <v>830</v>
+        <v>853</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>831</v>
+        <v>854</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="30"/>
@@ -12848,11 +13052,11 @@
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="30" t="s">
-        <v>832</v>
+        <v>855</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="30" t="s">
-        <v>833</v>
+        <v>856</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -12907,12 +13111,12 @@
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
       <c r="B12" s="30" t="s">
-        <v>834</v>
+        <v>857</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="21" t="s">
-        <v>835</v>
+        <v>858</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -12967,14 +13171,14 @@
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="30" t="s">
-        <v>836</v>
+        <v>859</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>837</v>
+        <v>860</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="21" t="s">
-        <v>838</v>
+        <v>861</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -13031,10 +13235,10 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="30" t="s">
-        <v>839</v>
+        <v>862</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>840</v>
+        <v>863</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -13063,10 +13267,10 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="30" t="s">
-        <v>841</v>
+        <v>864</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>842</v>
+        <v>865</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -13095,10 +13299,10 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="30" t="s">
-        <v>843</v>
+        <v>866</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>844</v>
+        <v>867</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -13154,11 +13358,11 @@
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="30" t="s">
-        <v>845</v>
+        <v>868</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="21" t="s">
-        <v>846</v>
+        <v>869</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -13215,10 +13419,10 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="30" t="s">
-        <v>839</v>
+        <v>862</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>847</v>
+        <v>870</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -13247,10 +13451,10 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="30" t="s">
-        <v>848</v>
+        <v>871</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>849</v>
+        <v>872</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -13306,11 +13510,11 @@
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="30" t="s">
-        <v>850</v>
+        <v>873</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="21" t="s">
-        <v>851</v>
+        <v>874</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -13367,10 +13571,10 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="31" t="s">
-        <v>852</v>
+        <v>875</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>853</v>
+        <v>876</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -13399,10 +13603,10 @@
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="31" t="s">
-        <v>854</v>
+        <v>877</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>855</v>
+        <v>878</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -13431,10 +13635,10 @@
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="31" t="s">
-        <v>856</v>
+        <v>879</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>857</v>
+        <v>880</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -13463,10 +13667,10 @@
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="31" t="s">
-        <v>858</v>
+        <v>881</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>859</v>
+        <v>882</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -13495,10 +13699,10 @@
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="31" t="s">
-        <v>860</v>
+        <v>883</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>861</v>
+        <v>884</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -13554,11 +13758,11 @@
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="30" t="s">
-        <v>862</v>
+        <v>885</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="21" t="s">
-        <v>863</v>
+        <v>886</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -13615,10 +13819,10 @@
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="30" t="s">
-        <v>839</v>
+        <v>862</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>864</v>
+        <v>887</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -13647,10 +13851,10 @@
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="30" t="s">
-        <v>865</v>
+        <v>888</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>866</v>
+        <v>889</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -13679,10 +13883,10 @@
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="30" t="s">
-        <v>867</v>
+        <v>890</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>868</v>
+        <v>891</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -13711,10 +13915,10 @@
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="30" t="s">
-        <v>869</v>
+        <v>892</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>870</v>
+        <v>893</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -13743,10 +13947,10 @@
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="30" t="s">
-        <v>871</v>
+        <v>894</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>872</v>
+        <v>895</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -13802,11 +14006,11 @@
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>873</v>
+        <v>896</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="21" t="s">
-        <v>874</v>
+        <v>897</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -13863,10 +14067,10 @@
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="30" t="s">
-        <v>839</v>
+        <v>862</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>875</v>
+        <v>898</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -13895,10 +14099,10 @@
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="31" t="s">
-        <v>876</v>
+        <v>899</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>877</v>
+        <v>900</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -13927,10 +14131,10 @@
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="30" t="s">
-        <v>878</v>
+        <v>901</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>879</v>
+        <v>902</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -13985,14 +14189,14 @@
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="30"/>
       <c r="B47" s="30" t="s">
-        <v>880</v>
+        <v>903</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>881</v>
+        <v>904</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="21" t="s">
-        <v>882</v>
+        <v>905</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
@@ -14022,7 +14226,7 @@
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
       <c r="E48" s="21" t="s">
-        <v>883</v>
+        <v>906</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
@@ -14052,7 +14256,7 @@
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
       <c r="E49" s="21" t="s">
-        <v>884</v>
+        <v>907</v>
       </c>
       <c r="F49" s="30"/>
       <c r="G49" s="30"/>
@@ -15089,7 +15293,7 @@
         <v>236</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>885</v>
+        <v>908</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>237</v>
@@ -15109,7 +15313,7 @@
         <v>273</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>886</v>
+        <v>909</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>210</v>
@@ -15129,7 +15333,7 @@
         <v>285</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>887</v>
+        <v>910</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>237</v>
@@ -15149,7 +15353,7 @@
         <v>432</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>888</v>
+        <v>911</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>306</v>
@@ -15166,7 +15370,7 @@
         <v>513</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>889</v>
+        <v>912</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>306</v>
@@ -15183,7 +15387,7 @@
         <v>400</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>890</v>
+        <v>913</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>306</v>
@@ -15200,7 +15404,7 @@
         <v>404</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>890</v>
+        <v>913</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>306</v>
@@ -15217,7 +15421,7 @@
         <v>413</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>891</v>
+        <v>914</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>306</v>
@@ -15225,16 +15429,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>892</v>
+        <v>915</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>893</v>
+        <v>916</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>894</v>
+        <v>917</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>895</v>
+        <v>918</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>306</v>
@@ -15251,7 +15455,7 @@
         <v>373</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>896</v>
+        <v>919</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>306</v>
@@ -15265,10 +15469,10 @@
         <v>436</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>897</v>
+        <v>920</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>898</v>
+        <v>921</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>306</v>
@@ -15276,16 +15480,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>899</v>
+        <v>922</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>900</v>
+        <v>923</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>901</v>
+        <v>924</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>902</v>
+        <v>925</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>306</v>
@@ -15293,16 +15497,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>903</v>
+        <v>926</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>904</v>
+        <v>927</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>905</v>
+        <v>928</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>906</v>
+        <v>929</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>306</v>
@@ -15319,7 +15523,7 @@
         <v>778</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>907</v>
+        <v>930</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>306</v>
@@ -15336,7 +15540,7 @@
         <v>746</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>908</v>
+        <v>931</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>237</v>
@@ -15356,7 +15560,7 @@
         <v>751</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>909</v>
+        <v>932</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>306</v>
@@ -15441,7 +15645,7 @@
         <v>572</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>910</v>
+        <v>933</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>237</v>
@@ -15461,7 +15665,7 @@
         <v>507</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>911</v>
+        <v>934</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>237</v>
@@ -15524,16 +15728,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>912</v>
+        <v>935</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>913</v>
+        <v>936</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>914</v>
+        <v>937</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>915</v>
+        <v>938</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -15544,16 +15748,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>916</v>
+        <v>939</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>917</v>
+        <v>940</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>918</v>
+        <v>941</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>919</v>
+        <v>942</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -15564,22 +15768,22 @@
     </row>
     <row r="4" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>920</v>
+        <v>943</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>921</v>
+        <v>944</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>922</v>
+        <v>945</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>923</v>
+        <v>946</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>924</v>
+        <v>947</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15593,7 +15797,7 @@
         <v>481</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>925</v>
+        <v>948</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -15604,16 +15808,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>926</v>
+        <v>949</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>927</v>
+        <v>950</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>928</v>
+        <v>951</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>929</v>
+        <v>952</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -15621,19 +15825,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>930</v>
+        <v>953</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>931</v>
+        <v>954</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>932</v>
+        <v>955</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>933</v>
+        <v>956</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>931</v>
+        <v>954</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15717,16 +15921,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>934</v>
+        <v>957</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>935</v>
+        <v>958</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>936</v>
+        <v>959</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>937</v>
+        <v>960</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -15734,42 +15938,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>938</v>
+        <v>961</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>939</v>
+        <v>962</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>940</v>
+        <v>963</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>941</v>
+        <v>964</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>942</v>
+        <v>965</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>943</v>
+        <v>966</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>944</v>
+        <v>967</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>945</v>
+        <v>968</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>946</v>
+        <v>969</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>947</v>
+        <v>970</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added missing state quantity
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="972">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -3091,6 +3091,9 @@
   </si>
   <si>
     <t xml:space="preserve">The value at which principal is being repaid. This may be including or excluding of interest depending on the Contract Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of shares / notes / certificates / etc in circulation</t>
   </si>
   <si>
     <t xml:space="preserve">The timestamp at which a contingent event/obligation is exercised</t>
@@ -3619,7 +3622,7 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5545,9 +5548,9 @@
   <dimension ref="A1:AF133"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15247,7 +15250,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -15529,103 +15532,103 @@
         <v>306</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>743</v>
+        <v>516</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>745</v>
+        <v>517</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>746</v>
+        <v>518</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>931</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>238</v>
+        <v>812</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>932</v>
       </c>
       <c r="E17" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>933</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>306</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
-        <v>809</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>810</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>811</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>813</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>814</v>
+        <v>809</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>815</v>
+        <v>810</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>816</v>
+        <v>811</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>812</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>818</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>819</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>820</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>821</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>306</v>
+      <c r="A20" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>821</v>
@@ -15634,43 +15637,60 @@
         <v>306</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>822</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>823</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>821</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
         <v>570</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B23" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>572</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>933</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="D23" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F23" s="0" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>505</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B24" s="0" t="s">
         <v>506</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C24" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>934</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="D24" s="0" t="s">
+        <v>935</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F24" s="0" t="s">
         <v>238</v>
       </c>
     </row>
@@ -15728,16 +15748,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -15748,16 +15768,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -15768,22 +15788,22 @@
     </row>
     <row r="4" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15797,7 +15817,7 @@
         <v>481</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -15808,16 +15828,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -15825,19 +15845,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>956</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>957</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>955</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>956</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15921,16 +15941,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -15938,42 +15958,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added missing states related to coupon payments
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="978">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -3106,6 +3106,24 @@
   </si>
   <si>
     <t xml:space="preserve">The timestamp as per which the contract matures according to the initial terms or as per unscheduled events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastCouponDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Coupon Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The most recent Coupon Day as per which the last Coupon Amount was fixed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Coupon Amount fixed with the last Coupon Fixing Day event and applicable to the next Coupon Payment Day event.</t>
   </si>
   <si>
     <t xml:space="preserve">eventTime</t>
@@ -5548,9 +5566,9 @@
   <dimension ref="A1:AF133"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
+      <selection pane="bottomLeft" activeCell="A133" activeCellId="0" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15250,10 +15268,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15692,6 +15710,43 @@
       </c>
       <c r="F24" s="0" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>937</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>939</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>845</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>941</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>306</v>
       </c>
     </row>
   </sheetData>
@@ -15748,16 +15803,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>936</v>
+        <v>942</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>937</v>
+        <v>943</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>938</v>
+        <v>944</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>939</v>
+        <v>945</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -15768,16 +15823,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>940</v>
+        <v>946</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>941</v>
+        <v>947</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>942</v>
+        <v>948</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>943</v>
+        <v>949</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -15788,22 +15843,22 @@
     </row>
     <row r="4" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>944</v>
+        <v>950</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>945</v>
+        <v>951</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>946</v>
+        <v>952</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>947</v>
+        <v>953</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>948</v>
+        <v>954</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15817,7 +15872,7 @@
         <v>481</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>949</v>
+        <v>955</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -15828,16 +15883,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>950</v>
+        <v>956</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>951</v>
+        <v>957</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>952</v>
+        <v>958</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>953</v>
+        <v>959</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -15845,19 +15900,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>954</v>
+        <v>960</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>955</v>
+        <v>961</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>956</v>
+        <v>962</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>957</v>
+        <v>963</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>955</v>
+        <v>961</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15941,16 +15996,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>958</v>
+        <v>964</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>959</v>
+        <v>965</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>960</v>
+        <v>966</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>961</v>
+        <v>967</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -15958,42 +16013,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>962</v>
+        <v>968</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>963</v>
+        <v>969</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>964</v>
+        <v>970</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>965</v>
+        <v>971</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>966</v>
+        <v>972</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>967</v>
+        <v>973</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>968</v>
+        <v>974</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>969</v>
+        <v>975</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>970</v>
+        <v>976</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>971</v>
+        <v>977</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added missing redemption day related events
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -3162,7 +3162,7 @@
     <t xml:space="preserve">The type of the event. Different types have their own business logic in terms of payoff and state transition functions</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 27
+    <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 28
 option: 1, identifier: issueDay, name: Issue Day, acronym: ID, description: Marks the day or timestamp respectively of issuance of a contract, sequence: 1
 option: 2, identifier: initialExchange, name: Initial Exchange, acronym: IED, description: Scheduled date of initial exchange of e.g. principal value in fixed income products, sequence: 2
 option: 3, identifier: feePayment, name: Fee Payment, acronym: FP, description: Scheduled fee payments, sequence: 3
@@ -3185,10 +3185,11 @@
 option: 20, identifier: maturity, name: Maturity, acronym: MD, description: Maturity of a contract, sequence: 20
 option: 21, identifier: couponFixingDay, name: Coupon Fixing Day, acronym: CFD, description: Fixing of the coupon amount, sequence: 21 
 option: 22, identifier: couponPaymentDay, name: Coupon Payment Day, acronym: CPD, description: Payment of the coupon amount, sequence: 22
-option: 23, identifier: redemptionDay, name: Redemption Day, acronym: RD, description: Fixing of the redemption amount, sequence: 23
-option: 24, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 24
-option: 25, identifier: exerciseDay, name: Exercise Day, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 25
-Option: 26, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 26</t>
+option: 23, identifier: redemptionFixingDay, name: Redemption Fixing Day, acronym: RFD, description: Fixing of the redemption amount, sequence: 23 
+option: 24, identifier: redemptionPaymentDay, name: Redemption Payment Day, acronym: RPD, description: Payment of the redemption amount, sequence: 24
+option: 25, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 25
+option: 26, identifier: exerciseDay, name: Exercise Day, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 26
+Option: 27, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 27</t>
   </si>
   <si>
     <t xml:space="preserve">The currency in which the event payoff is scheduled</t>

</xml_diff>

<commit_message>
added missing term lastCouponDay
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2264" uniqueCount="978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="979">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2663,6 +2663,9 @@
     <t xml:space="preserve">cycleAnchorDateOfRedemption</t>
   </si>
   <si>
+    <t xml:space="preserve">Redemption</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cycle Anchor Date Of Redemption Day</t>
   </si>
   <si>
@@ -2844,6 +2847,18 @@
     <t xml:space="preserve">The coupon amount fixed at the most recent coupon day and due for payment.</t>
   </si>
   <si>
+    <t xml:space="preserve">lastCouponDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last Coupon Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The most recent Coupon Day as per which the last Coupon Amount was fixed.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute Applicability Rules</t>
   </si>
   <si>
@@ -3106,18 +3121,6 @@
   </si>
   <si>
     <t xml:space="preserve">The timestamp as per which the contract matures according to the initial terms or as per unscheduled events</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastCouponDay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Coupon Day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The most recent Coupon Day as per which the last Coupon Amount was fixed.</t>
   </si>
   <si>
     <t xml:space="preserve">CAF</t>
@@ -5564,12 +5567,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AF133"/>
+  <dimension ref="A1:AF134"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A133" activeCellId="0" sqref="A133"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12336,18 +12339,18 @@
       </c>
       <c r="AC119" s="19"/>
     </row>
-    <row r="120" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="19" t="s">
         <v>788</v>
       </c>
       <c r="B120" s="19" t="s">
-        <v>616</v>
+        <v>789</v>
       </c>
       <c r="C120" s="19" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D120" s="19" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="E120" s="19" t="s">
         <v>237</v>
@@ -12358,7 +12361,7 @@
       <c r="G120" s="19"/>
       <c r="H120" s="19"/>
       <c r="I120" s="19" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="AB120" s="0" t="s">
         <v>214</v>
@@ -12367,16 +12370,16 @@
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="19" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>616</v>
+        <v>789</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="D121" s="19" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="E121" s="19" t="s">
         <v>335</v>
@@ -12387,25 +12390,25 @@
       <c r="G121" s="19"/>
       <c r="H121" s="19"/>
       <c r="I121" s="19" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="AB121" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC121" s="19"/>
     </row>
-    <row r="122" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="19" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>616</v>
+        <v>789</v>
       </c>
       <c r="C122" s="19" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="D122" s="19" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="E122" s="19" t="s">
         <v>237</v>
@@ -12416,7 +12419,7 @@
       <c r="G122" s="19"/>
       <c r="H122" s="19"/>
       <c r="I122" s="19" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="AB122" s="0" t="s">
         <v>214</v>
@@ -12425,16 +12428,16 @@
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="19" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>616</v>
+        <v>789</v>
       </c>
       <c r="C123" s="19" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="D123" s="19" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="E123" s="19" t="s">
         <v>335</v>
@@ -12445,7 +12448,7 @@
       <c r="G123" s="19"/>
       <c r="H123" s="19"/>
       <c r="I123" s="19" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="AB123" s="0" t="s">
         <v>214</v>
@@ -12454,16 +12457,16 @@
     </row>
     <row r="124" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="19" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>744</v>
+        <v>789</v>
       </c>
       <c r="C124" s="19" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="D124" s="19" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="E124" s="19" t="s">
         <v>290</v>
@@ -12472,32 +12475,32 @@
         <v>291</v>
       </c>
       <c r="G124" s="19" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="H124" s="19"/>
       <c r="I124" s="19" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="AB124" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC124" s="19"/>
     </row>
-    <row r="125" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="19" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>744</v>
+        <v>789</v>
       </c>
       <c r="C125" s="19" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="D125" s="19" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="E125" s="19" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="F125" s="19"/>
       <c r="G125" s="19" t="n">
@@ -12505,7 +12508,7 @@
       </c>
       <c r="H125" s="19"/>
       <c r="I125" s="19" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="J125" s="19"/>
       <c r="K125" s="19"/>
@@ -12535,19 +12538,19 @@
     </row>
     <row r="126" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="19" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B126" s="19" t="s">
-        <v>744</v>
+        <v>789</v>
       </c>
       <c r="C126" s="19" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D126" s="19" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="E126" s="19" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="F126" s="19"/>
       <c r="G126" s="19" t="n">
@@ -12555,7 +12558,7 @@
       </c>
       <c r="H126" s="19"/>
       <c r="I126" s="19" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="J126" s="19"/>
       <c r="K126" s="19"/>
@@ -12585,16 +12588,16 @@
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>744</v>
+        <v>789</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="D127" s="0" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="E127" s="0" t="s">
         <v>306</v>
@@ -12603,7 +12606,7 @@
         <v>1</v>
       </c>
       <c r="I127" s="0" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="AB127" s="0" t="s">
         <v>214</v>
@@ -12611,16 +12614,16 @@
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>744</v>
+        <v>789</v>
       </c>
       <c r="C128" s="0" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="D128" s="0" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="E128" s="0" t="s">
         <v>306</v>
@@ -12629,7 +12632,7 @@
         <v>1</v>
       </c>
       <c r="I128" s="0" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="AB128" s="0" t="s">
         <v>214</v>
@@ -12637,16 +12640,16 @@
     </row>
     <row r="129" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="D129" s="0" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="E129" s="0" t="s">
         <v>237</v>
@@ -12655,7 +12658,7 @@
         <v>238</v>
       </c>
       <c r="I129" s="19" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="AB129" s="19" t="s">
         <v>338</v>
@@ -12663,16 +12666,16 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E130" s="0" t="s">
         <v>335</v>
@@ -12681,7 +12684,7 @@
         <v>336</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="AB130" s="19" t="s">
         <v>338</v>
@@ -12689,28 +12692,28 @@
     </row>
     <row r="131" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="E131" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F131" s="19" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="G131" s="0" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="I131" s="0" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="AB131" s="19" t="s">
         <v>452</v>
@@ -12718,16 +12721,16 @@
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="D132" s="0" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="E132" s="0" t="s">
         <v>306</v>
@@ -12736,7 +12739,7 @@
         <v>0</v>
       </c>
       <c r="I132" s="0" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="AB132" s="19" t="s">
         <v>331</v>
@@ -12744,16 +12747,16 @@
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D133" s="0" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="E133" s="0" t="s">
         <v>306</v>
@@ -12762,9 +12765,35 @@
         <v>0</v>
       </c>
       <c r="I133" s="0" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="AB133" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>849</v>
+      </c>
+      <c r="B134" s="0" t="s">
+        <v>827</v>
+      </c>
+      <c r="C134" s="0" t="s">
+        <v>850</v>
+      </c>
+      <c r="D134" s="0" t="s">
+        <v>851</v>
+      </c>
+      <c r="E134" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="F134" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="I134" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="AB134" s="19" t="s">
         <v>338</v>
       </c>
     </row>
@@ -12835,7 +12864,7 @@
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="30" t="s">
-        <v>848</v>
+        <v>853</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -12893,7 +12922,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30"/>
       <c r="B4" s="30" t="s">
-        <v>849</v>
+        <v>854</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -12951,10 +12980,10 @@
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30"/>
       <c r="B6" s="30" t="s">
-        <v>850</v>
+        <v>855</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>851</v>
+        <v>856</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="30"/>
@@ -12984,7 +13013,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="30" t="s">
-        <v>852</v>
+        <v>857</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -13041,10 +13070,10 @@
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30"/>
       <c r="B9" s="30" t="s">
-        <v>853</v>
+        <v>858</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>854</v>
+        <v>859</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="30"/>
@@ -13074,11 +13103,11 @@
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="30" t="s">
-        <v>855</v>
+        <v>860</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="30" t="s">
-        <v>856</v>
+        <v>861</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -13133,12 +13162,12 @@
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
       <c r="B12" s="30" t="s">
-        <v>857</v>
+        <v>862</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="21" t="s">
-        <v>858</v>
+        <v>863</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -13193,14 +13222,14 @@
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="30" t="s">
-        <v>859</v>
+        <v>864</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>860</v>
+        <v>865</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="21" t="s">
-        <v>861</v>
+        <v>866</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -13257,10 +13286,10 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="30" t="s">
-        <v>862</v>
+        <v>867</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>863</v>
+        <v>868</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -13289,10 +13318,10 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="30" t="s">
-        <v>864</v>
+        <v>869</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>865</v>
+        <v>870</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -13321,10 +13350,10 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="30" t="s">
-        <v>866</v>
+        <v>871</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>867</v>
+        <v>872</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -13380,11 +13409,11 @@
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="30" t="s">
-        <v>868</v>
+        <v>873</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="21" t="s">
-        <v>869</v>
+        <v>874</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -13441,10 +13470,10 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="30" t="s">
-        <v>862</v>
+        <v>867</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>870</v>
+        <v>875</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -13473,10 +13502,10 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="30" t="s">
-        <v>871</v>
+        <v>876</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>872</v>
+        <v>877</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -13532,11 +13561,11 @@
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="30" t="s">
-        <v>873</v>
+        <v>878</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="21" t="s">
-        <v>874</v>
+        <v>879</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -13593,10 +13622,10 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="31" t="s">
-        <v>875</v>
+        <v>880</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>876</v>
+        <v>881</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -13625,10 +13654,10 @@
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="31" t="s">
-        <v>877</v>
+        <v>882</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>878</v>
+        <v>883</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -13657,10 +13686,10 @@
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="31" t="s">
-        <v>879</v>
+        <v>884</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>880</v>
+        <v>885</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -13689,10 +13718,10 @@
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="31" t="s">
-        <v>881</v>
+        <v>886</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>882</v>
+        <v>887</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -13721,10 +13750,10 @@
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="31" t="s">
-        <v>883</v>
+        <v>888</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>884</v>
+        <v>889</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -13780,11 +13809,11 @@
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="30" t="s">
-        <v>885</v>
+        <v>890</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="21" t="s">
-        <v>886</v>
+        <v>891</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -13841,10 +13870,10 @@
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="30" t="s">
-        <v>862</v>
+        <v>867</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>887</v>
+        <v>892</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -13873,10 +13902,10 @@
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="30" t="s">
-        <v>888</v>
+        <v>893</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>889</v>
+        <v>894</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -13905,10 +13934,10 @@
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="30" t="s">
-        <v>890</v>
+        <v>895</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>891</v>
+        <v>896</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -13937,10 +13966,10 @@
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="30" t="s">
-        <v>892</v>
+        <v>897</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>893</v>
+        <v>898</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -13969,10 +13998,10 @@
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="30" t="s">
-        <v>894</v>
+        <v>899</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>895</v>
+        <v>900</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -14028,11 +14057,11 @@
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>896</v>
+        <v>901</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="21" t="s">
-        <v>897</v>
+        <v>902</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -14089,10 +14118,10 @@
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="30" t="s">
-        <v>862</v>
+        <v>867</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>898</v>
+        <v>903</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -14121,10 +14150,10 @@
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="31" t="s">
-        <v>899</v>
+        <v>904</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>900</v>
+        <v>905</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -14153,10 +14182,10 @@
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="30" t="s">
-        <v>901</v>
+        <v>906</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>902</v>
+        <v>907</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -14211,14 +14240,14 @@
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="30"/>
       <c r="B47" s="30" t="s">
-        <v>903</v>
+        <v>908</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>904</v>
+        <v>909</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="21" t="s">
-        <v>905</v>
+        <v>910</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
@@ -14248,7 +14277,7 @@
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
       <c r="E48" s="21" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
@@ -14278,7 +14307,7 @@
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
       <c r="E49" s="21" t="s">
-        <v>907</v>
+        <v>912</v>
       </c>
       <c r="F49" s="30"/>
       <c r="G49" s="30"/>
@@ -15272,7 +15301,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15315,7 +15344,7 @@
         <v>236</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>908</v>
+        <v>913</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>237</v>
@@ -15335,7 +15364,7 @@
         <v>273</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>909</v>
+        <v>914</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>210</v>
@@ -15355,7 +15384,7 @@
         <v>285</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>910</v>
+        <v>915</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>237</v>
@@ -15375,7 +15404,7 @@
         <v>432</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>911</v>
+        <v>916</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>306</v>
@@ -15392,7 +15421,7 @@
         <v>513</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>912</v>
+        <v>917</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>306</v>
@@ -15409,7 +15438,7 @@
         <v>400</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>306</v>
@@ -15426,7 +15455,7 @@
         <v>404</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>913</v>
+        <v>918</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>306</v>
@@ -15443,7 +15472,7 @@
         <v>413</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>914</v>
+        <v>919</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>306</v>
@@ -15451,16 +15480,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>916</v>
+        <v>921</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>917</v>
+        <v>922</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>918</v>
+        <v>923</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>306</v>
@@ -15477,7 +15506,7 @@
         <v>373</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>919</v>
+        <v>924</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>306</v>
@@ -15491,10 +15520,10 @@
         <v>436</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>920</v>
+        <v>925</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>921</v>
+        <v>926</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>306</v>
@@ -15502,16 +15531,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>922</v>
+        <v>927</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>923</v>
+        <v>928</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>924</v>
+        <v>929</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>925</v>
+        <v>930</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>306</v>
@@ -15519,16 +15548,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>926</v>
+        <v>931</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>927</v>
+        <v>932</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>928</v>
+        <v>933</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>929</v>
+        <v>934</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>306</v>
@@ -15545,7 +15574,7 @@
         <v>778</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>930</v>
+        <v>935</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>306</v>
@@ -15562,10 +15591,10 @@
         <v>518</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>931</v>
+        <v>936</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15579,7 +15608,7 @@
         <v>746</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>932</v>
+        <v>937</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>237</v>
@@ -15599,7 +15628,7 @@
         <v>751</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>933</v>
+        <v>938</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>306</v>
@@ -15607,50 +15636,50 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>813</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>306</v>
@@ -15658,16 +15687,16 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>823</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>825</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>822</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>823</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>824</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>821</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>306</v>
@@ -15684,7 +15713,7 @@
         <v>572</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>934</v>
+        <v>939</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>237</v>
@@ -15704,7 +15733,7 @@
         <v>507</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>935</v>
+        <v>940</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>237</v>
@@ -15715,16 +15744,16 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>936</v>
+        <v>849</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>937</v>
+        <v>850</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>938</v>
+        <v>851</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>939</v>
+        <v>852</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>237</v>
@@ -15735,16 +15764,16 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>306</v>
@@ -15804,16 +15833,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -15824,16 +15853,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -15844,22 +15873,22 @@
     </row>
     <row r="4" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15873,7 +15902,7 @@
         <v>481</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -15884,16 +15913,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -15901,19 +15930,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>964</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>962</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>963</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15997,16 +16026,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -16014,42 +16043,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fixed typo in fixingPeriod accronym
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -2488,10 +2488,10 @@
     <t xml:space="preserve">Fixing Period</t>
   </si>
   <si>
-    <t xml:space="preserve">RRFIX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest rate resets (adjustments) are usually fixed one or two days (usually Business Days) before the new rate applies (defined by the rate reset schedule). This field holds the period between fixing and application of a rate.</t>
+    <t xml:space="preserve">FIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjustments of external data points (variable rates, redemption amounts, etc.) are usually fixed one or two days (usually Business Days) before they are applied (the fixing day). This field holds the period between fixing and application of a data point.</t>
   </si>
   <si>
     <t xml:space="preserve">nextResetRate</t>
@@ -3643,7 +3643,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5569,7 +5569,7 @@
   </sheetPr>
   <dimension ref="A1:AF134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>

</xml_diff>

<commit_message>
added missing CERTF contract type option
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -774,7 +774,8 @@
 option: 14, identifier: future, name: Future, acronym: FUTUR, description: An agreement of exchanging an underlying instrument against a fixed price in the future. 
 option: 15, identifier: option, name: Option, acronym: OPTNS, description: Different types of options on buying an underlying instrument at a fixed price in the future. 
 option: 16, identifier: creditEnhancementGuarantee, name: Credit Enhancement Guarantee, acronym: CEG, description: A guarantee / letter of credit by a third party on the scheduled payment obligations of an underlying instrument 
-option: 17, identifier: creditEnhancementCollateral, name: Credit Enhancement Collateral, acronym: CEC, description: A collateral securing the scheduled payment obligations of an underlying instrument</t>
+option: 17, identifier: creditEnhancementCollateral, name: Credit Enhancement Collateral, acronym: CEC, description: A collateral securing the scheduled payment obligations of an underlying instrument
+option: 18, identifier: certificate, name: Certificate, acronym: CERTF, description: A certificate letting the buyer participate in the performance of an underlying instrument. Often comes with specific rights of redemption, termination, and also special features on the payoff.</t>
   </si>
   <si>
     <t xml:space="preserve">The ContractType is the most important information. It defines the cash flow generating pattern of a contract. The ContractType information in combination with a given state of the risk factors will produce a deterministic sequence of cash flows which are the basis of any financial analysis.</t>
@@ -3643,7 +3644,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5569,7 +5570,7 @@
   </sheetPr>
   <dimension ref="A1:AF134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>

</xml_diff>

<commit_message>
removed trailing space in eventType options
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -3189,7 +3189,7 @@
 option: 20, identifier: maturity, name: Maturity, acronym: MD, description: Maturity of a contract, sequence: 20
 option: 21, identifier: couponFixingDay, name: Coupon Fixing Day, acronym: CFD, description: Fixing of the coupon amount, sequence: 21 
 option: 22, identifier: couponPaymentDay, name: Coupon Payment Day, acronym: CPD, description: Payment of the coupon amount, sequence: 22
-option: 23, identifier: redemptionFixingDay, name: Redemption Fixing Day, acronym: RFD, description: Fixing of the redemption amount, sequence: 23 
+option: 23, identifier: redemptionFixingDay, name: Redemption Fixing Day, acronym: RFD, description: Fixing of the redemption amount, sequence: 23
 option: 24, identifier: redemptionPaymentDay, name: Redemption Payment Day, acronym: RPD, description: Payment of the redemption amount, sequence: 24
 option: 25, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 25
 option: 26, identifier: exerciseDay, name: Exercise Day, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 26
@@ -3644,7 +3644,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -15798,8 +15798,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fixed formatting error in contractType enum options
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -775,7 +775,7 @@
 option: 15, identifier: option, name: Option, acronym: OPTNS, description: Different types of options on buying an underlying instrument at a fixed price in the future. 
 option: 16, identifier: creditEnhancementGuarantee, name: Credit Enhancement Guarantee, acronym: CEG, description: A guarantee / letter of credit by a third party on the scheduled payment obligations of an underlying instrument 
 option: 17, identifier: creditEnhancementCollateral, name: Credit Enhancement Collateral, acronym: CEC, description: A collateral securing the scheduled payment obligations of an underlying instrument
-option: 18, identifier: certificate, name: Certificate, acronym: CERTF, description: A certificate letting the buyer participate in the performance of an underlying instrument. Often comes with specific rights of redemption, termination, and also special features on the payoff.</t>
+option: 18, identifier: certificate, name: Certificate, acronym: CERTF, description: A certificate letting the buyer participate in the performance of an underlying instrument. Often comes with specific rights of redemption and termination and also special features on the payoff.</t>
   </si>
   <si>
     <t xml:space="preserve">The ContractType is the most important information. It defines the cash flow generating pattern of a contract. The ContractType information in combination with a given state of the risk factors will produce a deterministic sequence of cash flows which are the basis of any financial analysis.</t>
@@ -3644,7 +3644,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -15798,7 +15798,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
aligned naming conventions for CERTF/STK features
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1046">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -1101,7 +1101,7 @@
     <t xml:space="preserve">Cycle Anchor Date Of Dividend</t>
   </si>
   <si>
-    <t xml:space="preserve">DANX</t>
+    <t xml:space="preserve">DIANX</t>
   </si>
   <si>
     <t xml:space="preserve">Date from which the dividend payment date schedule is calculated according to the cycle length. The first dividend payment event takes place on this anchor.</t>
@@ -1116,7 +1116,7 @@
     <t xml:space="preserve">Cycle Of Dividend</t>
   </si>
   <si>
-    <t xml:space="preserve">DCL</t>
+    <t xml:space="preserve">DICL</t>
   </si>
   <si>
     <t xml:space="preserve">Cycle</t>
@@ -1137,7 +1137,7 @@
     <t xml:space="preserve">Dividend Ex Date</t>
   </si>
   <si>
-    <t xml:space="preserve">DED</t>
+    <t xml:space="preserve">DIEX</t>
   </si>
   <si>
     <t xml:space="preserve">In case contract is traded between DVEX and next DV payment date (i.e. PRD&gt;DVEX &amp; PRD&lt;next DV payment date), then the old holder of the contract (previous to the trade) receives the next DV payment. In other words, the next DV payment is cancelled for the new (after the trade) holder of the contract.</t>
@@ -1152,7 +1152,7 @@
     <t xml:space="preserve">Dividend Payment Date</t>
   </si>
   <si>
-    <t xml:space="preserve">DPD</t>
+    <t xml:space="preserve">DIPD</t>
   </si>
   <si>
     <t xml:space="preserve">The timestamp of the next Dividend Payment Date if one has been announced.</t>
@@ -1164,7 +1164,7 @@
     <t xml:space="preserve">Dividend Payment Amount</t>
   </si>
   <si>
-    <t xml:space="preserve">DPA</t>
+    <t xml:space="preserve">DIPA</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
@@ -1182,7 +1182,7 @@
     <t xml:space="preserve">Dividend Record Period</t>
   </si>
   <si>
-    <t xml:space="preserve">DRP</t>
+    <t xml:space="preserve">DIRP</t>
   </si>
   <si>
     <t xml:space="preserve">The period according to which the Dividend Ex Date is scheduled. More specifically, the Dividend Ex Date is scheduled at Dividend Declaration Date, the time at which a dividend event is announced, plus DRP.</t>
@@ -1194,7 +1194,7 @@
     <t xml:space="preserve">Dividend Payment Period</t>
   </si>
   <si>
-    <t xml:space="preserve">DPP</t>
+    <t xml:space="preserve">DIPP</t>
   </si>
   <si>
     <t xml:space="preserve">The period according to which the Dividend Payment Date is scheduled. More specifically, the Dividend Payment Date is scheduled at Dividend Declaration Date, the time at which a dividend event is announced, plus DPP.</t>
@@ -1206,7 +1206,7 @@
     <t xml:space="preserve">Last Dividend Fixing Date</t>
   </si>
   <si>
-    <t xml:space="preserve">LDFD</t>
+    <t xml:space="preserve">LDIFD</t>
   </si>
   <si>
     <t xml:space="preserve">The timestamp of the last DF event.</t>
@@ -1823,7 +1823,7 @@
     <t xml:space="preserve">Split Settlement Period</t>
   </si>
   <si>
-    <t xml:space="preserve">SEP</t>
+    <t xml:space="preserve">SPSP</t>
   </si>
   <si>
     <t xml:space="preserve">The period according to which stock splits are scheduled.</t>
@@ -1835,7 +1835,7 @@
     <t xml:space="preserve">Split Ratio</t>
   </si>
   <si>
-    <t xml:space="preserve">SRA</t>
+    <t xml:space="preserve">SPR</t>
   </si>
   <si>
     <t xml:space="preserve">The ratio according to which a stock split is executed.</t>
@@ -2607,7 +2607,7 @@
     <t xml:space="preserve">Exercise Date</t>
   </si>
   <si>
-    <t xml:space="preserve">XD</t>
+    <t xml:space="preserve">EXD</t>
   </si>
   <si>
     <t xml:space="preserve">Date of exercising a contingent event/obligation such as a forward condition, optionality etc. The Exercise date marks the observed timestamp of fixing the contingent event and respective payment obligation not necessarily the timestamp of settling the obligation.</t>
@@ -2622,7 +2622,7 @@
     <t xml:space="preserve">Exercise Amount</t>
   </si>
   <si>
-    <t xml:space="preserve">XA</t>
+    <t xml:space="preserve">EXA</t>
   </si>
   <si>
     <t xml:space="preserve">The amount fixed at Exercise Date for a contingent event/obligation such as a forward condition, optionality etc. The Exercise Amount is fixed at Exercise Date but not settled yet. </t>
@@ -2697,7 +2697,7 @@
     <t xml:space="preserve">Issue Date</t>
   </si>
   <si>
-    <t xml:space="preserve">ID</t>
+    <t xml:space="preserve">ISD</t>
   </si>
   <si>
     <t xml:space="preserve">Defines the time of issuance of the contract. At this time, the contract transitions from e.g. the subscription phase into the execution phase.</t>
@@ -2709,7 +2709,7 @@
     <t xml:space="preserve">Nominal Price</t>
   </si>
   <si>
-    <t xml:space="preserve">NPR</t>
+    <t xml:space="preserve">NOPR</t>
   </si>
   <si>
     <t xml:space="preserve">The nominal price for a single certificate.</t>
@@ -2721,7 +2721,7 @@
     <t xml:space="preserve">Issue Price</t>
   </si>
   <si>
-    <t xml:space="preserve">IPR</t>
+    <t xml:space="preserve">ISPR</t>
   </si>
   <si>
     <t xml:space="preserve">The issue price for a single certificate as per Issue Day.</t>
@@ -2748,7 +2748,7 @@
     <t xml:space="preserve">Redeemable By Issuer</t>
   </si>
   <si>
-    <t xml:space="preserve">RBI</t>
+    <t xml:space="preserve">REBI</t>
   </si>
   <si>
     <t xml:space="preserve">option: 0, identifier: yes, name: Yes, acronym: Y, description: The instrument is redeemable by the issuer.
@@ -2765,7 +2765,7 @@
     <t xml:space="preserve">Redemption Record Period</t>
   </si>
   <si>
-    <t xml:space="preserve">RRP</t>
+    <t xml:space="preserve">RERP</t>
   </si>
   <si>
     <t xml:space="preserve">The period according to which the Redemption Ex Date is scheduled. More specifically, the Redemption Ex Date is scheduled at the Redemption Declaration Date, which is the time when redemption is announced, plus RRP.</t>
@@ -2777,7 +2777,7 @@
     <t xml:space="preserve">Redemption Payment Period</t>
   </si>
   <si>
-    <t xml:space="preserve">RPP</t>
+    <t xml:space="preserve">REPP</t>
   </si>
   <si>
     <t xml:space="preserve">The period according to which the Redemption Payment Date is scheduled. More specifically, the Redemption Payment Date is scheduled at Redemption Declaration Date, which is the time when a redemption event is announced, plus RPP.</t>
@@ -2789,7 +2789,7 @@
     <t xml:space="preserve">Redemption Ex Date</t>
   </si>
   <si>
-    <t xml:space="preserve">RED</t>
+    <t xml:space="preserve">REXD</t>
   </si>
   <si>
     <t xml:space="preserve">The timestamp of the next Redemption Ex Date event if one has been announced.</t>
@@ -2801,7 +2801,7 @@
     <t xml:space="preserve">Redemption Payment Date</t>
   </si>
   <si>
-    <t xml:space="preserve">RPD</t>
+    <t xml:space="preserve">REPD</t>
   </si>
   <si>
     <t xml:space="preserve">The timestamp of the next Redemption Payment Date event if one has been announced.</t>
@@ -2813,7 +2813,7 @@
     <t xml:space="preserve">Redemption Price</t>
   </si>
   <si>
-    <t xml:space="preserve">RPR</t>
+    <t xml:space="preserve">REPR</t>
   </si>
   <si>
     <t xml:space="preserve">The redemption price applicable to the next Redemption Payment Date event if one has been announced.</t>
@@ -2825,7 +2825,7 @@
     <t xml:space="preserve">Cycle Anchor Date Of Redemption Day</t>
   </si>
   <si>
-    <t xml:space="preserve">RDANX</t>
+    <t xml:space="preserve">REANX</t>
   </si>
   <si>
     <t xml:space="preserve">The start date of the Redemption Day schedule. i.e. this is the very first regular Redemption Day. After this day periodic Redemption Days are scheduled through the Cycle of Redemption Day.</t>
@@ -2837,7 +2837,7 @@
     <t xml:space="preserve">Cycle Of Redemption Day</t>
   </si>
   <si>
-    <t xml:space="preserve">RDCL</t>
+    <t xml:space="preserve">RECL</t>
   </si>
   <si>
     <t xml:space="preserve">The period according to which Redemption Days are scheduled.</t>
@@ -2873,7 +2873,7 @@
     <t xml:space="preserve">Exercise Period</t>
   </si>
   <si>
-    <t xml:space="preserve">XP</t>
+    <t xml:space="preserve">EXP</t>
   </si>
   <si>
     <t xml:space="preserve">0D</t>
@@ -2888,7 +2888,7 @@
     <t xml:space="preserve">Exercise Quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">XQ</t>
+    <t xml:space="preserve">EXQ</t>
   </si>
   <si>
     <t xml:space="preserve">Integer</t>
@@ -2903,7 +2903,7 @@
     <t xml:space="preserve">Exercise Quantity Ordered</t>
   </si>
   <si>
-    <t xml:space="preserve">XO</t>
+    <t xml:space="preserve">EXO</t>
   </si>
   <si>
     <t xml:space="preserve">The number of shares / notes / certificates / etc ordered for exercise. E.g. the number of certificates ordered for redemption as per a certain redemption day.</t>
@@ -2939,7 +2939,7 @@
     <t xml:space="preserve">Cycle Anchor Date Of Coupon</t>
   </si>
   <si>
-    <t xml:space="preserve">CPANX</t>
+    <t xml:space="preserve">COANX</t>
   </si>
   <si>
     <t xml:space="preserve">The start date of the Coupon Day schedule. i.e. this is the very first regular Coupon Day. After this day periodic Coupon Days are scheduled through the Cycle of Coupon Day.</t>
@@ -2951,7 +2951,7 @@
     <t xml:space="preserve">Cycle Of Coupon</t>
   </si>
   <si>
-    <t xml:space="preserve">CPCL</t>
+    <t xml:space="preserve">COCL</t>
   </si>
   <si>
     <t xml:space="preserve">The period according to which Coupon Days are scheduled.</t>
@@ -2963,7 +2963,7 @@
     <t xml:space="preserve">Coupon Type</t>
   </si>
   <si>
-    <t xml:space="preserve">CPTP</t>
+    <t xml:space="preserve">COTP</t>
   </si>
   <si>
     <t xml:space="preserve">option: 0, identifier: none, name: No Coupon, acronym: NOC, description: No coupon is paid.
@@ -2985,7 +2985,7 @@
     <t xml:space="preserve">Coupon Rate</t>
   </si>
   <si>
-    <t xml:space="preserve">CPRT</t>
+    <t xml:space="preserve">CORT</t>
   </si>
   <si>
     <t xml:space="preserve">The fixed coupon applicable (if any). Applies in conjunction with couponType=FIX (fixed).</t>
@@ -2997,7 +2997,7 @@
     <t xml:space="preserve">Coupon Amount Fixed</t>
   </si>
   <si>
-    <t xml:space="preserve">CPFX</t>
+    <t xml:space="preserve">COAF</t>
   </si>
   <si>
     <t xml:space="preserve">The coupon amount fixed at the most recent coupon day and due for payment.</t>
@@ -3009,7 +3009,7 @@
     <t xml:space="preserve">Last Coupon Fixing Date</t>
   </si>
   <si>
-    <t xml:space="preserve">LCD</t>
+    <t xml:space="preserve">LCOD</t>
   </si>
   <si>
     <t xml:space="preserve">The most recent Coupon Day as per which the last Coupon Amount was fixed.</t>
@@ -3261,6 +3261,9 @@
     <t xml:space="preserve">The multiplier being applied to interest cash flows</t>
   </si>
   <si>
+    <t xml:space="preserve">NPR</t>
+  </si>
+  <si>
     <t xml:space="preserve">The value at which principal is being repaid. This may be including or excluding of interest depending on the Contract Type</t>
   </si>
   <si>
@@ -3297,7 +3300,7 @@
     <t xml:space="preserve">Dividend Fixing Date</t>
   </si>
   <si>
-    <t xml:space="preserve">DFD</t>
+    <t xml:space="preserve">DIFD</t>
   </si>
   <si>
     <t xml:space="preserve">The timestamp of the next DF event (if scheduled).</t>
@@ -3315,7 +3318,7 @@
     <t xml:space="preserve">Split Settlement Date</t>
   </si>
   <si>
-    <t xml:space="preserve">SSD</t>
+    <t xml:space="preserve">SPSD</t>
   </si>
   <si>
     <t xml:space="preserve">The timestmap of the next SSD event (if scheduled).</t>
@@ -3366,58 +3369,12 @@
     <t xml:space="preserve">The type of the event. Different types have their own business logic in terms of payoff and state transition functions</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 33
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">option: 1, identifier: creditEvent, name: Credit Event, acronym: CE, description: Credit event of counterparty to a contract, sequence: 1
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">option: 2, identifier: issue, name: Issue, acronym: IS, description: Marks the date or timestamp respectively of issuance of a contract, sequence: 2
+    <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 33
+option: 1, identifier: creditEvent, name: Credit Event, acronym: CE, description: Credit event of counterparty to a contract, sequence: 1
+option: 2, identifier: issue, name: Issue, acronym: ISS, description: Marks the date or timestamp respectively of issuance of a contract, sequence: 2
 option: 3, identifier: initialExchange, name: Initial Exchange, acronym: IED, description: Scheduled date of initial exchange of e.g. principal value in fixed income products, sequence: 3
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">option: 4, identifier: purchase, name: Purchase, acronym: PRD, description: Purchase of a contract, sequence: 4
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">option: 5, identifier: feePayment, name: Fee Payment, acronym: FP, description: Scheduled fee payments, sequence: 5
+option: 4, identifier: purchase, name: Purchase, acronym: PRD, description: Purchase of a contract, sequence: 4
+option: 5, identifier: feePayment, name: Fee Payment, acronym: FP, description: Scheduled fee payments, sequence: 5
 option: 6, identifier: principalRedemption, name: Principal Redemption, acronym: PR, description: Scheduled principal redemption payment, sequence: 6
 option: 7, identifier: principalDrawing, name: Principal Drawing, acronym: PD, description: Drawing of principal amount e.g. in a credit line, sequence: 7
 option: 8, identifier: penaltyPayment, name: Penalty Payment, acronym: PY, description: Scheduled payment of a penalty, sequence: 8
@@ -3426,46 +3383,18 @@
 option: 11, identifier: interestCapitalization, name: Interest Capitalization, acronym: IPCI, description: Scheduled capitalization of accrued interest, sequence: 11
 option: 12, identifier: rateResetFixed, name: Rate Reset Fixing with Known Rate, acronym: RRF, description: Scheduled fixing of variable rate with known new rate, sequence: 12
 option: 13, identifier: rateResetVariable, name: Rate Reset Fixing with Unknown Rate, acronym: RR, description: Scheduled fixing of variable rate with unknown new rate, sequence: 13
-option: 14, identifier: dividendFixing, name: Dividend Fixing, acronym: DF, description: Declaration of a dividend payment, sequence: 14
-option: 15, identifier: dividendEx, name: Dividend Ex, acronym: DE, description: Date from which new shareholders are not considered for the next dividend distribution, sequence: 15
-option: 16, identifier: dividendPayment, name: Dividend Payment, acronym: DP, description: Date at which next dividend is distributed to shareholders, sequence: 16
-option: 17, identifier: couponFixing, name: Coupon Fixing, acronym: CF, description: Fixing of the coupon amount, sequence: 17
-option: 18, identifier: couponPayment, name: Coupon Payment, acronym: CP, description: Payment of the coupon amount, sequence: 18
-option: 19, identifier: redemptionFixing, name: Redemption Fixing, acronym: RF, description: Fixing of the redemption amount, sequence: 19
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">option: 20, identifier: redemptionEx, name: Redemption Ex, acronym: RE, description: Date from which new holders are not considered for next redemption, sequence: 20
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">option: 21, identifier: redemptionPayment, name: Redemption Payment, acronym: RP, description: Payment of the redemption amount, sequence: 21
-option: 22, identifier: splitDeclaration, name: Split Declaration, acronym: SD, description: Declaration of a stock split or reverse split, sequence: 22
-option: 23, identifier: splitSettlement, name: Split Settlement, acronym: SE, description: Date at which stock split is settled or settlement is finalized, sequence: 23
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">option: 24, identifier: exerciseOrder, name: Exercise Order, acronym: XO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 24
-option: 25, identifier: exercise, name: Exercise, acronym: XE, description: Exercise of a contractual feature such as an optionality, sequence: 25
+option: 14, identifier: dividendFixing, name: Dividend Fixing, acronym: DIF, description: Declaration of a dividend payment, sequence: 14
+option: 15, identifier: dividendEx, name: Dividend Ex, acronym: DIX, description: Date from which new shareholders are not considered for the next dividend distribution, sequence: 15
+option: 16, identifier: dividendPayment, name: Dividend Payment, acronym: DIP, description: Date at which next dividend is distributed to shareholders, sequence: 16
+option: 17, identifier: couponFixing, name: Coupon Fixing, acronym: COF, description: Fixing of the coupon amount, sequence: 17
+option: 18, identifier: couponPayment, name: Coupon Payment, acronym: COP, description: Payment of the coupon amount, sequence: 18
+option: 19, identifier: redemptionFixing, name: Redemption Fixing, acronym: REF, description: Fixing of the redemption amount, sequence: 19
+option: 20, identifier: redemptionEx, name: Redemption Ex, acronym: REX, description: Date from which new holders are not considered for next redemption, sequence: 20
+option: 21, identifier: redemptionPayment, name: Redemption Payment, acronym: REP, description: Payment of the redemption amount, sequence: 21
+option: 22, identifier: splitFixing, name: Split Fixing, acronym: SPF, description: Declaration of a stock split or reverse split, sequence: 22
+option: 23, identifier: splitSettlement, name: Split Settlement, acronym: SPS, description: Date at which stock split is settled or settlement is finalized, sequence: 23
+option: 24, identifier: exerciseOrder, name: Exercise Order, acronym: EXO, description: Submission of an exercise order for a contractual feature such as an optionality, sequence: 24
+option: 25, identifier: exercise, name: Exercise, acronym: EXE, description: Exercise of a contractual feature such as an optionality, sequence: 25
 option: 26, identifier: settlement, name: Settlement, acronym: ST, description: Settlement of an exercised contractual claim, sequence: 26
 option: 27, identifier: scalingIndexFixing, name: Scaling Index Fixing, acronym: SC, description: Scheduled fixing of a scaling index, sequence: 27
 option: 28, identifier: interestCalculationBaseFixing, name: Interest Calculation Base Fixing, acronym: IPCB, description: Scheduled fixing of the interest calculation base, sequence: 28
@@ -3474,7 +3403,6 @@
 option: 31, identifier: termination, name: Termination, acronym: TD, description: Termination of a contract, sequence: 31
 option: 32, identifier: maturity, name: Maturity, acronym: MD, description: Maturity of a contract, sequence: 32
 </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">The currency in which the event payoff is scheduled</t>
@@ -3563,7 +3491,7 @@
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3686,12 +3614,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -16034,7 +15956,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16304,10 +16226,10 @@
         <v>571</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>804</v>
+        <v>986</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>306</v>
@@ -16324,7 +16246,7 @@
         <v>534</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>864</v>
@@ -16341,7 +16263,7 @@
         <v>772</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>237</v>
@@ -16361,7 +16283,7 @@
         <v>777</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>306</v>
@@ -16446,7 +16368,7 @@
         <v>596</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>237</v>
@@ -16466,7 +16388,7 @@
         <v>523</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>237</v>
@@ -16483,10 +16405,10 @@
         <v>901</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>237</v>
@@ -16503,10 +16425,10 @@
         <v>897</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>306</v>
@@ -16534,16 +16456,16 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>237</v>
@@ -16563,7 +16485,7 @@
         <v>346</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>237</v>
@@ -16583,7 +16505,7 @@
         <v>350</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>306</v>
@@ -16591,16 +16513,16 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>237</v>
@@ -16620,7 +16542,7 @@
         <v>548</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>306</v>
@@ -16640,7 +16562,7 @@
         <v>830</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>237</v>
@@ -16660,7 +16582,7 @@
         <v>834</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>237</v>
@@ -16688,8 +16610,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16725,16 +16647,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -16745,16 +16667,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1015</v>
+        <v>1016</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -16765,22 +16687,22 @@
     </row>
     <row r="4" customFormat="false" ht="501.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1018</v>
+        <v>1019</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1019</v>
+        <v>1020</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16794,7 +16716,7 @@
         <v>497</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -16805,16 +16727,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -16822,19 +16744,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>1029</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>1030</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>1028</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16918,16 +16840,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -16935,42 +16857,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fixed redemption exercise period naming conventions
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -2783,6 +2783,21 @@
     <t xml:space="preserve">The period according to which the Redemption Payment Date is scheduled. More specifically, the Redemption Payment Date is scheduled at Redemption Declaration Date, which is the time when a redemption event is announced, plus RPP.</t>
   </si>
   <si>
+    <t xml:space="preserve">redemptionExercisePeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redemption Exercise Period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REXP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The period within which an option holder (e.g. from redemption of a note / certificate / etc) can chose to execute his option</t>
+  </si>
+  <si>
     <t xml:space="preserve">redemptionExDate</t>
   </si>
   <si>
@@ -2865,21 +2880,6 @@
   </si>
   <si>
     <t xml:space="preserve">The period according to which Termination Days are scheduled.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exercisePeriod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exercise Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The period within which an option holder (e.g. from redemption of a note / certificate / etc) can chose to execute his option</t>
   </si>
   <si>
     <t xml:space="preserve">exerciseQuantity</t>
@@ -5777,12 +5777,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AF146"/>
+  <dimension ref="A1:AF1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12916,45 +12916,49 @@
       </c>
       <c r="AC128" s="19"/>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+    <row r="129" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="19" t="s">
         <v>828</v>
       </c>
-      <c r="B129" s="0" t="s">
+      <c r="B129" s="19" t="s">
         <v>815</v>
       </c>
-      <c r="C129" s="0" t="s">
+      <c r="C129" s="19" t="s">
         <v>829</v>
       </c>
-      <c r="D129" s="0" t="s">
+      <c r="D129" s="19" t="s">
         <v>830</v>
       </c>
-      <c r="E129" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="F129" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="I129" s="0" t="s">
+      <c r="E129" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="F129" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="G129" s="19" t="s">
         <v>831</v>
       </c>
-      <c r="R129" s="0" t="s">
+      <c r="H129" s="19"/>
+      <c r="I129" s="19" t="s">
+        <v>832</v>
+      </c>
+      <c r="AB129" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC129" s="19"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>815</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="D130" s="0" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E130" s="0" t="s">
         <v>237</v>
@@ -12963,7 +12967,7 @@
         <v>238</v>
       </c>
       <c r="I130" s="0" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="R130" s="0" t="s">
         <v>214</v>
@@ -12972,166 +12976,162 @@
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>815</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="D131" s="0" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="E131" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="F131" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="I131" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="R131" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC131" s="19"/>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>841</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>842</v>
+      </c>
+      <c r="D132" s="0" t="s">
+        <v>843</v>
+      </c>
+      <c r="E132" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="I131" s="0" t="s">
-        <v>839</v>
-      </c>
-      <c r="R131" s="0" t="s">
+      <c r="I132" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="R132" s="0" t="s">
         <v>616</v>
       </c>
-      <c r="AC131" s="19"/>
-    </row>
-    <row r="132" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="19" t="s">
-        <v>840</v>
-      </c>
-      <c r="B132" s="19" t="s">
-        <v>815</v>
-      </c>
-      <c r="C132" s="19" t="s">
-        <v>841</v>
-      </c>
-      <c r="D132" s="19" t="s">
-        <v>842</v>
-      </c>
-      <c r="E132" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="F132" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="G132" s="19"/>
-      <c r="H132" s="19"/>
-      <c r="I132" s="19" t="s">
-        <v>843</v>
-      </c>
-      <c r="AB132" s="0" t="s">
-        <v>214</v>
-      </c>
       <c r="AC132" s="19"/>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="19" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B133" s="19" t="s">
         <v>815</v>
       </c>
       <c r="C133" s="19" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D133" s="19" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="E133" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="F133" s="19" t="s">
-        <v>336</v>
+        <v>237</v>
+      </c>
+      <c r="F133" s="21" t="s">
+        <v>238</v>
       </c>
       <c r="G133" s="19"/>
       <c r="H133" s="19"/>
       <c r="I133" s="19" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="AB133" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC133" s="19"/>
     </row>
-    <row r="134" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="19" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="B134" s="19" t="s">
         <v>815</v>
       </c>
       <c r="C134" s="19" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="D134" s="19" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="E134" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="F134" s="21" t="s">
-        <v>238</v>
+        <v>335</v>
+      </c>
+      <c r="F134" s="19" t="s">
+        <v>336</v>
       </c>
       <c r="G134" s="19"/>
       <c r="H134" s="19"/>
       <c r="I134" s="19" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="AB134" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC134" s="19"/>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="19" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="B135" s="19" t="s">
         <v>815</v>
       </c>
       <c r="C135" s="19" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="D135" s="19" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="E135" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="F135" s="19" t="s">
-        <v>336</v>
+        <v>237</v>
+      </c>
+      <c r="F135" s="21" t="s">
+        <v>238</v>
       </c>
       <c r="G135" s="19"/>
       <c r="H135" s="19"/>
       <c r="I135" s="19" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="AB135" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC135" s="19"/>
     </row>
-    <row r="136" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="19" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B136" s="19" t="s">
         <v>815</v>
       </c>
       <c r="C136" s="19" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="D136" s="19" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="E136" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="F136" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="G136" s="19" t="s">
-        <v>859</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="F136" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="G136" s="19"/>
       <c r="H136" s="19"/>
       <c r="I136" s="19" t="s">
         <v>860</v>
@@ -13452,6 +13452,7 @@
         <v>338</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="T1:T121"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -16553,13 +16554,13 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>828</v>
+        <v>833</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="D33" s="0" t="s">
         <v>1008</v>
@@ -16573,13 +16574,13 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>832</v>
+        <v>837</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>833</v>
+        <v>838</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>834</v>
+        <v>839</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>1009</v>

</xml_diff>

<commit_message>
fixed minor inconsistency in naming conventions
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1045">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -3282,13 +3282,10 @@
     <t xml:space="preserve">The timestamp as per which the contract matures according to the initial terms or as per unscheduled events</t>
   </si>
   <si>
-    <t xml:space="preserve">LCFD</t>
+    <t xml:space="preserve">LCOFD</t>
   </si>
   <si>
     <t xml:space="preserve">The timestamp of the last CF event.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAF</t>
   </si>
   <si>
     <t xml:space="preserve">The Coupon Amount fixed with the last Coupon Fixing Day event and applicable to the next Coupon Payment Day event.</t>
@@ -5780,9 +5777,9 @@
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15957,7 +15954,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16426,10 +16423,10 @@
         <v>897</v>
       </c>
       <c r="C26" s="0" t="s">
+        <v>898</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>995</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>996</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>306</v>
@@ -16457,16 +16454,16 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>996</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>997</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="C28" s="0" t="s">
         <v>998</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="D28" s="0" t="s">
         <v>999</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>1000</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>237</v>
@@ -16486,7 +16483,7 @@
         <v>346</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>237</v>
@@ -16506,7 +16503,7 @@
         <v>350</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>306</v>
@@ -16514,16 +16511,16 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>1003</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="C31" s="0" t="s">
         <v>1004</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>1005</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>1006</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>237</v>
@@ -16543,7 +16540,7 @@
         <v>548</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>306</v>
@@ -16563,7 +16560,7 @@
         <v>835</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>237</v>
@@ -16583,7 +16580,7 @@
         <v>839</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>237</v>
@@ -16648,16 +16645,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>1010</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>1011</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>1012</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>1013</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -16668,16 +16665,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>1014</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>1015</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>1016</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>1017</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -16688,22 +16685,22 @@
     </row>
     <row r="4" customFormat="false" ht="501.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>1018</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>1019</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>1020</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>1021</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16717,7 +16714,7 @@
         <v>497</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -16728,16 +16725,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>1024</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>1025</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>1026</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>1027</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -16745,19 +16742,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>1028</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>1029</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>1030</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>1031</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16841,16 +16838,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>1032</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>1033</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>1034</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>1035</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -16858,42 +16855,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>1036</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>1037</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>1038</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>1039</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>1041</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>1042</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>1043</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>1044</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added ISS term to PAM,LAM,NAM,LAX
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2425" uniqueCount="1045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="1040">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2781,21 +2781,6 @@
   </si>
   <si>
     <t xml:space="preserve">The period according to which the Redemption Payment Date is scheduled. More specifically, the Redemption Payment Date is scheduled at Redemption Declaration Date, which is the time when a redemption event is announced, plus RPP.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">redemptionExercisePeriod</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redemption Exercise Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REXP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The period within which an option holder (e.g. from redemption of a note / certificate / etc) can chose to execute his option</t>
   </si>
   <si>
     <t xml:space="preserve">redemptionExDate</t>
@@ -3849,7 +3834,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5775,7 +5760,7 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -9417,19 +9402,19 @@
         <v>233</v>
       </c>
       <c r="M61" s="19" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="N61" s="19" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="O61" s="19" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="P61" s="19" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="Q61" s="19" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="R61" s="27"/>
       <c r="S61" s="22"/>
@@ -12725,6 +12710,21 @@
       <c r="I122" s="19" t="s">
         <v>801</v>
       </c>
+      <c r="M122" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="N122" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="O122" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="P122" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q122" s="0" t="s">
+        <v>233</v>
+      </c>
       <c r="R122" s="0" t="s">
         <v>233</v>
       </c>
@@ -12822,7 +12822,7 @@
       </c>
       <c r="AC125" s="19"/>
     </row>
-    <row r="126" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>814</v>
       </c>
@@ -12880,6 +12880,9 @@
       <c r="R127" s="0" t="s">
         <v>214</v>
       </c>
+      <c r="AB127" s="0" t="s">
+        <v>214</v>
+      </c>
       <c r="AC127" s="19"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12910,33 +12913,35 @@
       <c r="R128" s="0" t="s">
         <v>214</v>
       </c>
+      <c r="AB128" s="0" t="s">
+        <v>214</v>
+      </c>
       <c r="AC128" s="19"/>
     </row>
-    <row r="129" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="19" t="s">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
         <v>828</v>
       </c>
-      <c r="B129" s="19" t="s">
+      <c r="B129" s="0" t="s">
         <v>815</v>
       </c>
-      <c r="C129" s="19" t="s">
+      <c r="C129" s="0" t="s">
         <v>829</v>
       </c>
-      <c r="D129" s="19" t="s">
+      <c r="D129" s="0" t="s">
         <v>830</v>
       </c>
-      <c r="E129" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="F129" s="24" t="s">
-        <v>291</v>
-      </c>
-      <c r="G129" s="19" t="s">
+      <c r="E129" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="F129" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="I129" s="0" t="s">
         <v>831</v>
       </c>
-      <c r="H129" s="19"/>
-      <c r="I129" s="19" t="s">
-        <v>832</v>
+      <c r="R129" s="0" t="s">
+        <v>214</v>
       </c>
       <c r="AB129" s="0" t="s">
         <v>214</v>
@@ -12945,16 +12950,16 @@
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="B130" s="0" t="s">
         <v>815</v>
       </c>
       <c r="C130" s="0" t="s">
+        <v>833</v>
+      </c>
+      <c r="D130" s="0" t="s">
         <v>834</v>
-      </c>
-      <c r="D130" s="0" t="s">
-        <v>835</v>
       </c>
       <c r="E130" s="0" t="s">
         <v>237</v>
@@ -12963,179 +12968,208 @@
         <v>238</v>
       </c>
       <c r="I130" s="0" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="R130" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB130" s="0" t="s">
         <v>214</v>
       </c>
       <c r="AC130" s="19"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="B131" s="0" t="s">
         <v>815</v>
       </c>
       <c r="C131" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="D131" s="0" t="s">
         <v>838</v>
       </c>
-      <c r="D131" s="0" t="s">
+      <c r="E131" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="I131" s="0" t="s">
         <v>839</v>
       </c>
-      <c r="E131" s="0" t="s">
+      <c r="R131" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="AB131" s="0" t="s">
+        <v>616</v>
+      </c>
+      <c r="AC131" s="19"/>
+    </row>
+    <row r="132" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="19" t="s">
+        <v>840</v>
+      </c>
+      <c r="B132" s="19" t="s">
+        <v>815</v>
+      </c>
+      <c r="C132" s="19" t="s">
+        <v>841</v>
+      </c>
+      <c r="D132" s="19" t="s">
+        <v>842</v>
+      </c>
+      <c r="E132" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="F131" s="0" t="s">
+      <c r="F132" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="I131" s="0" t="s">
-        <v>840</v>
-      </c>
-      <c r="R131" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC131" s="19"/>
-    </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
-        <v>841</v>
-      </c>
-      <c r="B132" s="0" t="s">
-        <v>815</v>
-      </c>
-      <c r="C132" s="0" t="s">
-        <v>842</v>
-      </c>
-      <c r="D132" s="0" t="s">
+      <c r="G132" s="19"/>
+      <c r="H132" s="19"/>
+      <c r="I132" s="19" t="s">
         <v>843</v>
       </c>
-      <c r="E132" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="I132" s="0" t="s">
+      <c r="AB132" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC132" s="19"/>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="19" t="s">
         <v>844</v>
-      </c>
-      <c r="R132" s="0" t="s">
-        <v>616</v>
-      </c>
-      <c r="AC132" s="19"/>
-    </row>
-    <row r="133" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="19" t="s">
-        <v>845</v>
       </c>
       <c r="B133" s="19" t="s">
         <v>815</v>
       </c>
       <c r="C133" s="19" t="s">
+        <v>845</v>
+      </c>
+      <c r="D133" s="19" t="s">
         <v>846</v>
       </c>
-      <c r="D133" s="19" t="s">
-        <v>847</v>
-      </c>
       <c r="E133" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="F133" s="21" t="s">
-        <v>238</v>
+        <v>335</v>
+      </c>
+      <c r="F133" s="19" t="s">
+        <v>336</v>
       </c>
       <c r="G133" s="19"/>
       <c r="H133" s="19"/>
       <c r="I133" s="19" t="s">
+        <v>847</v>
+      </c>
+      <c r="AB133" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC133" s="19"/>
+    </row>
+    <row r="134" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="19" t="s">
         <v>848</v>
-      </c>
-      <c r="AB133" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC133" s="19"/>
-    </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="19" t="s">
-        <v>849</v>
       </c>
       <c r="B134" s="19" t="s">
         <v>815</v>
       </c>
       <c r="C134" s="19" t="s">
+        <v>849</v>
+      </c>
+      <c r="D134" s="19" t="s">
         <v>850</v>
       </c>
-      <c r="D134" s="19" t="s">
-        <v>851</v>
-      </c>
       <c r="E134" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="F134" s="19" t="s">
-        <v>336</v>
+        <v>237</v>
+      </c>
+      <c r="F134" s="21" t="s">
+        <v>238</v>
       </c>
       <c r="G134" s="19"/>
       <c r="H134" s="19"/>
       <c r="I134" s="19" t="s">
+        <v>851</v>
+      </c>
+      <c r="AB134" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC134" s="19"/>
+    </row>
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="19" t="s">
         <v>852</v>
-      </c>
-      <c r="AB134" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC134" s="19"/>
-    </row>
-    <row r="135" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="19" t="s">
-        <v>853</v>
       </c>
       <c r="B135" s="19" t="s">
         <v>815</v>
       </c>
       <c r="C135" s="19" t="s">
+        <v>853</v>
+      </c>
+      <c r="D135" s="19" t="s">
         <v>854</v>
       </c>
-      <c r="D135" s="19" t="s">
-        <v>855</v>
-      </c>
       <c r="E135" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="F135" s="21" t="s">
-        <v>238</v>
+        <v>335</v>
+      </c>
+      <c r="F135" s="19" t="s">
+        <v>336</v>
       </c>
       <c r="G135" s="19"/>
       <c r="H135" s="19"/>
       <c r="I135" s="19" t="s">
+        <v>855</v>
+      </c>
+      <c r="AB135" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC135" s="19"/>
+    </row>
+    <row r="136" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="19" t="s">
         <v>856</v>
-      </c>
-      <c r="AB135" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC135" s="19"/>
-    </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="19" t="s">
-        <v>857</v>
       </c>
       <c r="B136" s="19" t="s">
         <v>815</v>
       </c>
       <c r="C136" s="19" t="s">
+        <v>857</v>
+      </c>
+      <c r="D136" s="19" t="s">
         <v>858</v>
       </c>
-      <c r="D136" s="19" t="s">
+      <c r="E136" s="19" t="s">
         <v>859</v>
       </c>
-      <c r="E136" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="F136" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="G136" s="19"/>
+      <c r="F136" s="19"/>
+      <c r="G136" s="19" t="n">
+        <v>0</v>
+      </c>
       <c r="H136" s="19"/>
       <c r="I136" s="19" t="s">
         <v>860</v>
       </c>
-      <c r="AB136" s="0" t="s">
+      <c r="J136" s="19"/>
+      <c r="K136" s="19"/>
+      <c r="L136" s="19"/>
+      <c r="M136" s="19"/>
+      <c r="N136" s="19"/>
+      <c r="O136" s="19"/>
+      <c r="P136" s="19"/>
+      <c r="Q136" s="19"/>
+      <c r="R136" s="19"/>
+      <c r="S136" s="19"/>
+      <c r="T136" s="19"/>
+      <c r="U136" s="19"/>
+      <c r="V136" s="19"/>
+      <c r="W136" s="19"/>
+      <c r="X136" s="19"/>
+      <c r="Y136" s="19"/>
+      <c r="Z136" s="19"/>
+      <c r="AA136" s="19"/>
+      <c r="AB136" s="19" t="s">
         <v>214</v>
       </c>
       <c r="AC136" s="19"/>
+      <c r="AD136" s="19"/>
+      <c r="AE136" s="19"/>
+      <c r="AF136" s="19"/>
     </row>
     <row r="137" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="19" t="s">
@@ -13151,7 +13185,7 @@
         <v>863</v>
       </c>
       <c r="E137" s="19" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="F137" s="19"/>
       <c r="G137" s="19" t="n">
@@ -13159,7 +13193,7 @@
       </c>
       <c r="H137" s="19"/>
       <c r="I137" s="19" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="J137" s="19"/>
       <c r="K137" s="19"/>
@@ -13187,68 +13221,44 @@
       <c r="AE137" s="19"/>
       <c r="AF137" s="19"/>
     </row>
-    <row r="138" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="19" t="s">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="B138" s="0" t="s">
+        <v>815</v>
+      </c>
+      <c r="C138" s="0" t="s">
         <v>866</v>
       </c>
-      <c r="B138" s="19" t="s">
-        <v>815</v>
-      </c>
-      <c r="C138" s="19" t="s">
+      <c r="D138" s="0" t="s">
         <v>867</v>
       </c>
-      <c r="D138" s="19" t="s">
+      <c r="E138" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="G138" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I138" s="0" t="s">
         <v>868</v>
       </c>
-      <c r="E138" s="19" t="s">
-        <v>864</v>
-      </c>
-      <c r="F138" s="19"/>
-      <c r="G138" s="19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H138" s="19"/>
-      <c r="I138" s="19" t="s">
-        <v>869</v>
-      </c>
-      <c r="J138" s="19"/>
-      <c r="K138" s="19"/>
-      <c r="L138" s="19"/>
-      <c r="M138" s="19"/>
-      <c r="N138" s="19"/>
-      <c r="O138" s="19"/>
-      <c r="P138" s="19"/>
-      <c r="Q138" s="19"/>
-      <c r="R138" s="19"/>
-      <c r="S138" s="19"/>
-      <c r="T138" s="19"/>
-      <c r="U138" s="19"/>
-      <c r="V138" s="19"/>
-      <c r="W138" s="19"/>
-      <c r="X138" s="19"/>
-      <c r="Y138" s="19"/>
-      <c r="Z138" s="19"/>
-      <c r="AA138" s="19"/>
-      <c r="AB138" s="19" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC138" s="19"/>
-      <c r="AD138" s="19"/>
-      <c r="AE138" s="19"/>
-      <c r="AF138" s="19"/>
+      <c r="AB138" s="0" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B139" s="0" t="s">
         <v>815</v>
       </c>
       <c r="C139" s="0" t="s">
+        <v>870</v>
+      </c>
+      <c r="D139" s="0" t="s">
         <v>871</v>
-      </c>
-      <c r="D139" s="0" t="s">
-        <v>872</v>
       </c>
       <c r="E139" s="0" t="s">
         <v>306</v>
@@ -13257,131 +13267,131 @@
         <v>1</v>
       </c>
       <c r="I139" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="AB139" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="B140" s="0" t="s">
         <v>873</v>
       </c>
-      <c r="AB139" s="0" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+      <c r="C140" s="0" t="s">
         <v>874</v>
       </c>
-      <c r="B140" s="0" t="s">
-        <v>815</v>
-      </c>
-      <c r="C140" s="0" t="s">
+      <c r="D140" s="0" t="s">
         <v>875</v>
       </c>
-      <c r="D140" s="0" t="s">
+      <c r="E140" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="F140" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="I140" s="19" t="s">
         <v>876</v>
       </c>
-      <c r="E140" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="G140" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I140" s="0" t="s">
-        <v>873</v>
-      </c>
-      <c r="AB140" s="0" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB140" s="19" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>877</v>
       </c>
       <c r="B141" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="C141" s="0" t="s">
         <v>878</v>
       </c>
-      <c r="C141" s="0" t="s">
+      <c r="D141" s="0" t="s">
         <v>879</v>
       </c>
-      <c r="D141" s="0" t="s">
+      <c r="E141" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="F141" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="I141" s="19" t="s">
         <v>880</v>
-      </c>
-      <c r="E141" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="F141" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="I141" s="19" t="s">
-        <v>881</v>
       </c>
       <c r="AB141" s="19" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
+        <v>881</v>
+      </c>
+      <c r="B142" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="C142" s="0" t="s">
         <v>882</v>
       </c>
-      <c r="B142" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="C142" s="0" t="s">
+      <c r="D142" s="0" t="s">
         <v>883</v>
       </c>
-      <c r="D142" s="0" t="s">
+      <c r="E142" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="F142" s="19" t="s">
         <v>884</v>
       </c>
-      <c r="E142" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="F142" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="I142" s="19" t="s">
+      <c r="G142" s="0" t="s">
         <v>885</v>
       </c>
+      <c r="I142" s="0" t="s">
+        <v>886</v>
+      </c>
       <c r="AB142" s="19" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="169.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="D143" s="0" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="E143" s="0" t="s">
-        <v>210</v>
-      </c>
-      <c r="F143" s="19" t="s">
-        <v>889</v>
-      </c>
-      <c r="G143" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="G143" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I143" s="0" t="s">
         <v>890</v>
       </c>
-      <c r="I143" s="0" t="s">
-        <v>891</v>
-      </c>
       <c r="AB143" s="19" t="s">
-        <v>468</v>
+        <v>331</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
+        <v>891</v>
+      </c>
+      <c r="B144" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="C144" s="0" t="s">
         <v>892</v>
       </c>
-      <c r="B144" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="C144" s="0" t="s">
+      <c r="D144" s="0" t="s">
         <v>893</v>
-      </c>
-      <c r="D144" s="0" t="s">
-        <v>894</v>
       </c>
       <c r="E144" s="0" t="s">
         <v>306</v>
@@ -13390,64 +13400,39 @@
         <v>0</v>
       </c>
       <c r="I144" s="0" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="AB144" s="19" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
+        <v>895</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="C145" s="0" t="s">
         <v>896</v>
       </c>
-      <c r="B145" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="C145" s="0" t="s">
+      <c r="D145" s="0" t="s">
         <v>897</v>
       </c>
-      <c r="D145" s="0" t="s">
+      <c r="E145" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="F145" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="I145" s="0" t="s">
         <v>898</v>
-      </c>
-      <c r="E145" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="G145" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I145" s="0" t="s">
-        <v>899</v>
       </c>
       <c r="AB145" s="19" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
-        <v>900</v>
-      </c>
-      <c r="B146" s="0" t="s">
-        <v>878</v>
-      </c>
-      <c r="C146" s="0" t="s">
-        <v>901</v>
-      </c>
-      <c r="D146" s="0" t="s">
-        <v>902</v>
-      </c>
-      <c r="E146" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="F146" s="0" t="s">
-        <v>238</v>
-      </c>
-      <c r="I146" s="0" t="s">
-        <v>903</v>
-      </c>
-      <c r="AB146" s="19" t="s">
-        <v>338</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="T1:T121"/>
@@ -13516,7 +13501,7 @@
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="30" t="s">
-        <v>904</v>
+        <v>899</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -13574,7 +13559,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30"/>
       <c r="B4" s="30" t="s">
-        <v>905</v>
+        <v>900</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -13632,10 +13617,10 @@
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30"/>
       <c r="B6" s="30" t="s">
-        <v>906</v>
+        <v>901</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>907</v>
+        <v>902</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="30"/>
@@ -13665,7 +13650,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="30" t="s">
-        <v>908</v>
+        <v>903</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -13722,10 +13707,10 @@
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30"/>
       <c r="B9" s="30" t="s">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>910</v>
+        <v>905</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="30"/>
@@ -13755,11 +13740,11 @@
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="30" t="s">
-        <v>911</v>
+        <v>906</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="30" t="s">
-        <v>912</v>
+        <v>907</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -13814,12 +13799,12 @@
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
       <c r="B12" s="30" t="s">
-        <v>913</v>
+        <v>908</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="21" t="s">
-        <v>914</v>
+        <v>909</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -13874,14 +13859,14 @@
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="30" t="s">
-        <v>915</v>
+        <v>910</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>916</v>
+        <v>911</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="21" t="s">
-        <v>917</v>
+        <v>912</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -13938,10 +13923,10 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="30" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>919</v>
+        <v>914</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -13970,10 +13955,10 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="30" t="s">
-        <v>920</v>
+        <v>915</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>921</v>
+        <v>916</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -14002,10 +13987,10 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="30" t="s">
-        <v>922</v>
+        <v>917</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>923</v>
+        <v>918</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -14061,11 +14046,11 @@
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="30" t="s">
-        <v>924</v>
+        <v>919</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="21" t="s">
-        <v>925</v>
+        <v>920</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -14122,10 +14107,10 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="30" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>926</v>
+        <v>921</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -14154,10 +14139,10 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="30" t="s">
-        <v>927</v>
+        <v>922</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>928</v>
+        <v>923</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -14213,11 +14198,11 @@
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="30" t="s">
-        <v>929</v>
+        <v>924</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="21" t="s">
-        <v>930</v>
+        <v>925</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -14274,10 +14259,10 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="31" t="s">
-        <v>931</v>
+        <v>926</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -14306,10 +14291,10 @@
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="31" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -14338,10 +14323,10 @@
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="31" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -14370,10 +14355,10 @@
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="31" t="s">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>938</v>
+        <v>933</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -14402,10 +14387,10 @@
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="31" t="s">
-        <v>939</v>
+        <v>934</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>940</v>
+        <v>935</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -14461,11 +14446,11 @@
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="30" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="21" t="s">
-        <v>942</v>
+        <v>937</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -14522,10 +14507,10 @@
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="30" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>943</v>
+        <v>938</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -14554,10 +14539,10 @@
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="30" t="s">
-        <v>944</v>
+        <v>939</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>945</v>
+        <v>940</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -14586,10 +14571,10 @@
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="30" t="s">
-        <v>946</v>
+        <v>941</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -14618,10 +14603,10 @@
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="30" t="s">
-        <v>948</v>
+        <v>943</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>949</v>
+        <v>944</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -14650,10 +14635,10 @@
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="30" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>951</v>
+        <v>946</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -14709,11 +14694,11 @@
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>952</v>
+        <v>947</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="21" t="s">
-        <v>953</v>
+        <v>948</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -14770,10 +14755,10 @@
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="30" t="s">
-        <v>918</v>
+        <v>913</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>954</v>
+        <v>949</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -14802,10 +14787,10 @@
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="31" t="s">
-        <v>955</v>
+        <v>950</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>956</v>
+        <v>951</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -14834,10 +14819,10 @@
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="30" t="s">
-        <v>957</v>
+        <v>952</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>958</v>
+        <v>953</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -14892,14 +14877,14 @@
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="30"/>
       <c r="B47" s="30" t="s">
-        <v>959</v>
+        <v>954</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>960</v>
+        <v>955</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="21" t="s">
-        <v>961</v>
+        <v>956</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
@@ -14929,7 +14914,7 @@
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
       <c r="E48" s="21" t="s">
-        <v>962</v>
+        <v>957</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
@@ -14959,7 +14944,7 @@
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
       <c r="E49" s="21" t="s">
-        <v>963</v>
+        <v>958</v>
       </c>
       <c r="F49" s="30"/>
       <c r="G49" s="30"/>
@@ -15953,7 +15938,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15996,7 +15981,7 @@
         <v>236</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>964</v>
+        <v>959</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>237</v>
@@ -16016,7 +16001,7 @@
         <v>273</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>965</v>
+        <v>960</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>210</v>
@@ -16036,7 +16021,7 @@
         <v>285</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>966</v>
+        <v>961</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>237</v>
@@ -16056,7 +16041,7 @@
         <v>448</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>967</v>
+        <v>962</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>306</v>
@@ -16073,7 +16058,7 @@
         <v>529</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>968</v>
+        <v>963</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>306</v>
@@ -16090,7 +16075,7 @@
         <v>416</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>969</v>
+        <v>964</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>306</v>
@@ -16107,7 +16092,7 @@
         <v>420</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>969</v>
+        <v>964</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>306</v>
@@ -16124,7 +16109,7 @@
         <v>429</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>970</v>
+        <v>965</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>306</v>
@@ -16132,16 +16117,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>971</v>
+        <v>966</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>972</v>
+        <v>967</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>973</v>
+        <v>968</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>974</v>
+        <v>969</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>306</v>
@@ -16158,7 +16143,7 @@
         <v>389</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>975</v>
+        <v>970</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>306</v>
@@ -16172,10 +16157,10 @@
         <v>452</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>976</v>
+        <v>971</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>977</v>
+        <v>972</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>306</v>
@@ -16183,16 +16168,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>978</v>
+        <v>973</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>979</v>
+        <v>974</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>980</v>
+        <v>975</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>981</v>
+        <v>976</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>306</v>
@@ -16200,16 +16185,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>982</v>
+        <v>977</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>983</v>
+        <v>978</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>984</v>
+        <v>979</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>985</v>
+        <v>980</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>306</v>
@@ -16223,10 +16208,10 @@
         <v>571</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>986</v>
+        <v>981</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>987</v>
+        <v>982</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>306</v>
@@ -16243,10 +16228,10 @@
         <v>534</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>988</v>
+        <v>983</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16260,7 +16245,7 @@
         <v>772</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>989</v>
+        <v>984</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>237</v>
@@ -16280,7 +16265,7 @@
         <v>777</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>990</v>
+        <v>985</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>306</v>
@@ -16288,50 +16273,50 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>870</v>
+        <v>865</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>871</v>
+        <v>866</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>872</v>
+        <v>867</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>306</v>
@@ -16339,16 +16324,16 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>874</v>
+        <v>869</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>875</v>
+        <v>870</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>876</v>
+        <v>871</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>873</v>
+        <v>868</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>306</v>
@@ -16365,7 +16350,7 @@
         <v>596</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>991</v>
+        <v>986</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>237</v>
@@ -16385,7 +16370,7 @@
         <v>523</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>992</v>
+        <v>987</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>237</v>
@@ -16396,16 +16381,16 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>900</v>
+        <v>895</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>901</v>
+        <v>896</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>993</v>
+        <v>988</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>994</v>
+        <v>989</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>237</v>
@@ -16416,16 +16401,16 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>896</v>
+        <v>891</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>897</v>
+        <v>892</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>898</v>
+        <v>893</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>995</v>
+        <v>990</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>306</v>
@@ -16453,16 +16438,16 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>996</v>
+        <v>991</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>997</v>
+        <v>992</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>998</v>
+        <v>993</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>999</v>
+        <v>994</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>237</v>
@@ -16482,7 +16467,7 @@
         <v>346</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>237</v>
@@ -16502,7 +16487,7 @@
         <v>350</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1001</v>
+        <v>996</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>306</v>
@@ -16510,16 +16495,16 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>1002</v>
+        <v>997</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>1003</v>
+        <v>998</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>1004</v>
+        <v>999</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>1005</v>
+        <v>1000</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>237</v>
@@ -16539,7 +16524,7 @@
         <v>548</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1006</v>
+        <v>1001</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>306</v>
@@ -16550,16 +16535,16 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>1007</v>
+        <v>1002</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>237</v>
@@ -16570,16 +16555,16 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>1008</v>
+        <v>1003</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>237</v>
@@ -16644,16 +16629,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1009</v>
+        <v>1004</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1010</v>
+        <v>1005</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1011</v>
+        <v>1006</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1012</v>
+        <v>1007</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
@@ -16664,16 +16649,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1013</v>
+        <v>1008</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1014</v>
+        <v>1009</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1015</v>
+        <v>1010</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1016</v>
+        <v>1011</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
@@ -16684,22 +16669,22 @@
     </row>
     <row r="4" customFormat="false" ht="501.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1017</v>
+        <v>1012</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1018</v>
+        <v>1013</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1019</v>
+        <v>1014</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1020</v>
+        <v>1015</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>1021</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16713,7 +16698,7 @@
         <v>497</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1022</v>
+        <v>1017</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -16724,16 +16709,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1023</v>
+        <v>1018</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1024</v>
+        <v>1019</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1025</v>
+        <v>1020</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1026</v>
+        <v>1021</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -16741,19 +16726,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1027</v>
+        <v>1022</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1028</v>
+        <v>1023</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>1029</v>
+        <v>1024</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1030</v>
+        <v>1025</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1028</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16837,16 +16822,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1031</v>
+        <v>1026</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1032</v>
+        <v>1027</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1033</v>
+        <v>1028</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1034</v>
+        <v>1029</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -16854,42 +16839,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1035</v>
+        <v>1030</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1036</v>
+        <v>1031</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1037</v>
+        <v>1032</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1038</v>
+        <v>1033</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>1039</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1040</v>
+        <v>1035</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1041</v>
+        <v>1036</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1042</v>
+        <v>1037</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1043</v>
+        <v>1038</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>1044</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added collateral terms and cleaned up issues
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2426" uniqueCount="1040">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2485" uniqueCount="1055">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2998,6 +2998,51 @@
   </si>
   <si>
     <t xml:space="preserve">The most recent Coupon Day as per which the last Coupon Amount was fixed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collateralCurrency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collateral Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COCU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The currency of the collateral to be supplied for securing a contract.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x(10,1,)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coverageOfCollateral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coverage Of Collateral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(0,Infinity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The coverage of contract nominal value that the collateral must maintain. i.e. if coverageOfCollateral=0.5 the market value of the collateral must always be higher than 50% of the nominal value of the contract.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x(10,0,)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marketObjectCodeOfCollateral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market Object Code Of Collateral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The identifier of the market price feed of the collateral securing a contract.</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute Applicability Rules</t>
@@ -3666,7 +3711,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3788,6 +3833,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3834,7 +3883,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5760,7 +5809,7 @@
   </sheetPr>
   <dimension ref="A1:AF1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -13430,6 +13479,189 @@
       </c>
       <c r="AB145" s="19" t="s">
         <v>338</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="30" t="s">
+        <v>899</v>
+      </c>
+      <c r="B146" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>900</v>
+      </c>
+      <c r="D146" s="0" t="s">
+        <v>901</v>
+      </c>
+      <c r="E146" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="F146" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="I146" s="0" t="s">
+        <v>902</v>
+      </c>
+      <c r="M146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="N146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="O146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="P146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="Q146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="T146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="V146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="W146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="X146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="Y146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="Z146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="AA146" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="AB146" s="0" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="30" t="s">
+        <v>904</v>
+      </c>
+      <c r="B147" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>905</v>
+      </c>
+      <c r="D147" s="0" t="s">
+        <v>906</v>
+      </c>
+      <c r="E147" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="F147" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="I147" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="M147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="N147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="O147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="P147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="Q147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="T147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="V147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="W147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="X147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="Y147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="Z147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="AA147" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="AB147" s="0" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>910</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C148" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="D148" s="0" t="s">
+        <v>912</v>
+      </c>
+      <c r="E148" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="I148" s="0" t="s">
+        <v>913</v>
+      </c>
+      <c r="M148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="N148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="O148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="P148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="Q148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="T148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="V148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="W148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="X148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="Y148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="Z148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="AA148" s="0" t="s">
+        <v>903</v>
+      </c>
+      <c r="AB148" s="0" t="s">
+        <v>903</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -13471,37 +13703,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="30"/>
+      <c r="A1" s="31"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="30"/>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
-      <c r="B2" s="30" t="s">
-        <v>899</v>
+      <c r="B2" s="31" t="s">
+        <v>914</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -13523,10 +13755,10 @@
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30"/>
-      <c r="Z2" s="30"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
@@ -13551,40 +13783,40 @@
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="30"/>
-      <c r="Y3" s="30"/>
-      <c r="Z3" s="30"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30" t="s">
-        <v>900</v>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31" t="s">
+        <v>915</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
@@ -13610,47 +13842,47 @@
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
-      <c r="X5" s="30"/>
-      <c r="Y5" s="30"/>
-      <c r="Z5" s="30"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30" t="s">
-        <v>901</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>902</v>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31" t="s">
+        <v>916</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>917</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
+      <c r="Z6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="30" t="s">
-        <v>903</v>
+      <c r="C7" s="31" t="s">
+        <v>918</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -13672,9 +13904,9 @@
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
@@ -13700,51 +13932,51 @@
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30" t="s">
-        <v>904</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>905</v>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31" t="s">
+        <v>919</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>920</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="30" t="s">
-        <v>906</v>
+      <c r="C10" s="31" t="s">
+        <v>921</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="30" t="s">
-        <v>907</v>
+      <c r="E10" s="31" t="s">
+        <v>922</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -13766,7 +13998,7 @@
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
-      <c r="Z10" s="30"/>
+      <c r="Z10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
@@ -13794,17 +14026,17 @@
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
-      <c r="Z11" s="30"/>
+      <c r="Z11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
-      <c r="B12" s="30" t="s">
-        <v>908</v>
+      <c r="B12" s="31" t="s">
+        <v>923</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="21" t="s">
-        <v>909</v>
+        <v>924</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -13826,47 +14058,47 @@
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
-      <c r="Z12" s="30"/>
+      <c r="Z12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30"/>
+      <c r="A13" s="31"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30"/>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
-      <c r="B14" s="30" t="s">
-        <v>910</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>911</v>
+      <c r="B14" s="31" t="s">
+        <v>925</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>926</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="21" t="s">
-        <v>912</v>
+        <v>927</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -13888,7 +14120,7 @@
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
-      <c r="Z14" s="30"/>
+      <c r="Z14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
@@ -13916,17 +14148,17 @@
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
-      <c r="Z15" s="30"/>
+      <c r="Z15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="30" t="s">
-        <v>913</v>
+      <c r="D16" s="31" t="s">
+        <v>928</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>914</v>
+        <v>929</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -13948,17 +14180,17 @@
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
-      <c r="Z16" s="30"/>
+      <c r="Z16" s="31"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="30" t="s">
-        <v>915</v>
+      <c r="D17" s="31" t="s">
+        <v>930</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>916</v>
+        <v>931</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -13980,17 +14212,17 @@
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
-      <c r="Z17" s="30"/>
+      <c r="Z17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="30" t="s">
-        <v>917</v>
+      <c r="D18" s="31" t="s">
+        <v>932</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>918</v>
+        <v>933</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -14012,7 +14244,7 @@
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
       <c r="Y18" s="10"/>
-      <c r="Z18" s="30"/>
+      <c r="Z18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
@@ -14040,17 +14272,17 @@
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="10"/>
-      <c r="Z19" s="30"/>
+      <c r="Z19" s="31"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="30" t="s">
-        <v>919</v>
+      <c r="C20" s="31" t="s">
+        <v>934</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="21" t="s">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -14072,7 +14304,7 @@
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
       <c r="Y20" s="10"/>
-      <c r="Z20" s="30"/>
+      <c r="Z20" s="31"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
@@ -14100,17 +14332,17 @@
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="10"/>
-      <c r="Z21" s="30"/>
+      <c r="Z21" s="31"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="30" t="s">
-        <v>913</v>
+      <c r="D22" s="31" t="s">
+        <v>928</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>921</v>
+        <v>936</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -14132,17 +14364,17 @@
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
-      <c r="Z22" s="30"/>
+      <c r="Z22" s="31"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="30" t="s">
-        <v>922</v>
+      <c r="D23" s="31" t="s">
+        <v>937</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>923</v>
+        <v>938</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -14164,45 +14396,45 @@
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
-      <c r="Z23" s="30"/>
+      <c r="Z23" s="31"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="30"/>
+      <c r="A24" s="31"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="30"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
-      <c r="U24" s="30"/>
-      <c r="V24" s="30"/>
-      <c r="W24" s="30"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="30"/>
-      <c r="Z24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="31"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="31"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="30" t="s">
-        <v>924</v>
+      <c r="C25" s="31" t="s">
+        <v>939</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="21" t="s">
-        <v>925</v>
+        <v>940</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -14224,45 +14456,45 @@
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
-      <c r="Z25" s="30"/>
+      <c r="Z25" s="31"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="30"/>
+      <c r="A26" s="31"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
-      <c r="N26" s="30"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
-      <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
-      <c r="U26" s="30"/>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-      <c r="Y26" s="30"/>
-      <c r="Z26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="31"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="31"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="31" t="s">
-        <v>926</v>
+      <c r="D27" s="32" t="s">
+        <v>941</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>927</v>
+        <v>942</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -14284,17 +14516,17 @@
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
-      <c r="Z27" s="30"/>
+      <c r="Z27" s="31"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="31" t="s">
-        <v>928</v>
+      <c r="D28" s="32" t="s">
+        <v>943</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>929</v>
+        <v>944</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -14316,17 +14548,17 @@
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10"/>
-      <c r="Z28" s="30"/>
+      <c r="Z28" s="31"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="31" t="s">
-        <v>930</v>
+      <c r="D29" s="32" t="s">
+        <v>945</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>931</v>
+        <v>946</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -14348,17 +14580,17 @@
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
-      <c r="Z29" s="30"/>
+      <c r="Z29" s="31"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="31" t="s">
-        <v>932</v>
+      <c r="D30" s="32" t="s">
+        <v>947</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>933</v>
+        <v>948</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -14380,17 +14612,17 @@
       <c r="W30" s="10"/>
       <c r="X30" s="10"/>
       <c r="Y30" s="10"/>
-      <c r="Z30" s="30"/>
+      <c r="Z30" s="31"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
-      <c r="D31" s="31" t="s">
-        <v>934</v>
+      <c r="D31" s="32" t="s">
+        <v>949</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>935</v>
+        <v>950</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -14412,45 +14644,45 @@
       <c r="W31" s="10"/>
       <c r="X31" s="10"/>
       <c r="Y31" s="10"/>
-      <c r="Z31" s="30"/>
+      <c r="Z31" s="31"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="30"/>
-      <c r="V32" s="30"/>
-      <c r="W32" s="30"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="30"/>
-      <c r="Z32" s="30"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
+      <c r="X32" s="31"/>
+      <c r="Y32" s="31"/>
+      <c r="Z32" s="31"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
-      <c r="C33" s="30" t="s">
-        <v>936</v>
+      <c r="C33" s="31" t="s">
+        <v>951</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="21" t="s">
-        <v>937</v>
+        <v>952</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -14472,45 +14704,45 @@
       <c r="W33" s="10"/>
       <c r="X33" s="10"/>
       <c r="Y33" s="10"/>
-      <c r="Z33" s="30"/>
+      <c r="Z33" s="31"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="30"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="30"/>
-      <c r="Z34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
+      <c r="N34" s="31"/>
+      <c r="O34" s="31"/>
+      <c r="P34" s="31"/>
+      <c r="Q34" s="31"/>
+      <c r="R34" s="31"/>
+      <c r="S34" s="31"/>
+      <c r="T34" s="31"/>
+      <c r="U34" s="31"/>
+      <c r="V34" s="31"/>
+      <c r="W34" s="31"/>
+      <c r="X34" s="31"/>
+      <c r="Y34" s="31"/>
+      <c r="Z34" s="31"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="30" t="s">
-        <v>913</v>
+      <c r="D35" s="31" t="s">
+        <v>928</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>938</v>
+        <v>953</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -14532,17 +14764,17 @@
       <c r="W35" s="10"/>
       <c r="X35" s="10"/>
       <c r="Y35" s="10"/>
-      <c r="Z35" s="30"/>
+      <c r="Z35" s="31"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="30" t="s">
-        <v>939</v>
+      <c r="D36" s="31" t="s">
+        <v>954</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>940</v>
+        <v>955</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -14564,17 +14796,17 @@
       <c r="W36" s="10"/>
       <c r="X36" s="10"/>
       <c r="Y36" s="10"/>
-      <c r="Z36" s="30"/>
+      <c r="Z36" s="31"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="30" t="s">
-        <v>941</v>
+      <c r="D37" s="31" t="s">
+        <v>956</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>942</v>
+        <v>957</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -14596,17 +14828,17 @@
       <c r="W37" s="10"/>
       <c r="X37" s="10"/>
       <c r="Y37" s="10"/>
-      <c r="Z37" s="30"/>
+      <c r="Z37" s="31"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
-      <c r="D38" s="30" t="s">
-        <v>943</v>
+      <c r="D38" s="31" t="s">
+        <v>958</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>944</v>
+        <v>959</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -14628,17 +14860,17 @@
       <c r="W38" s="10"/>
       <c r="X38" s="10"/>
       <c r="Y38" s="10"/>
-      <c r="Z38" s="30"/>
+      <c r="Z38" s="31"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
-      <c r="D39" s="30" t="s">
-        <v>945</v>
+      <c r="D39" s="31" t="s">
+        <v>960</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>946</v>
+        <v>961</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -14660,7 +14892,7 @@
       <c r="W39" s="10"/>
       <c r="X39" s="10"/>
       <c r="Y39" s="10"/>
-      <c r="Z39" s="30"/>
+      <c r="Z39" s="31"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10"/>
@@ -14688,17 +14920,17 @@
       <c r="W40" s="10"/>
       <c r="X40" s="10"/>
       <c r="Y40" s="10"/>
-      <c r="Z40" s="30"/>
+      <c r="Z40" s="31"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>947</v>
+        <v>962</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="21" t="s">
-        <v>948</v>
+        <v>963</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -14720,7 +14952,7 @@
       <c r="W41" s="10"/>
       <c r="X41" s="10"/>
       <c r="Y41" s="10"/>
-      <c r="Z41" s="30"/>
+      <c r="Z41" s="31"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10"/>
@@ -14748,17 +14980,17 @@
       <c r="W42" s="10"/>
       <c r="X42" s="10"/>
       <c r="Y42" s="10"/>
-      <c r="Z42" s="30"/>
+      <c r="Z42" s="31"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
-      <c r="D43" s="30" t="s">
-        <v>913</v>
-      </c>
-      <c r="E43" s="30" t="s">
-        <v>949</v>
+      <c r="D43" s="31" t="s">
+        <v>928</v>
+      </c>
+      <c r="E43" s="31" t="s">
+        <v>964</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -14780,17 +15012,17 @@
       <c r="W43" s="10"/>
       <c r="X43" s="10"/>
       <c r="Y43" s="10"/>
-      <c r="Z43" s="30"/>
+      <c r="Z43" s="31"/>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
-      <c r="D44" s="31" t="s">
-        <v>950</v>
+      <c r="D44" s="32" t="s">
+        <v>965</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>951</v>
+        <v>966</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -14812,17 +15044,17 @@
       <c r="W44" s="10"/>
       <c r="X44" s="10"/>
       <c r="Y44" s="10"/>
-      <c r="Z44" s="30"/>
+      <c r="Z44" s="31"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
-      <c r="D45" s="30" t="s">
-        <v>952</v>
+      <c r="D45" s="31" t="s">
+        <v>967</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>953</v>
+        <v>968</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -14844,129 +15076,129 @@
       <c r="W45" s="10"/>
       <c r="X45" s="10"/>
       <c r="Y45" s="10"/>
-      <c r="Z45" s="30"/>
+      <c r="Z45" s="31"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="30"/>
+      <c r="A46" s="31"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
-      <c r="D46" s="30"/>
-      <c r="E46" s="30"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
-      <c r="K46" s="30"/>
-      <c r="L46" s="30"/>
-      <c r="M46" s="30"/>
-      <c r="N46" s="30"/>
-      <c r="O46" s="30"/>
-      <c r="P46" s="30"/>
-      <c r="Q46" s="30"/>
-      <c r="R46" s="30"/>
-      <c r="S46" s="30"/>
-      <c r="T46" s="30"/>
-      <c r="U46" s="30"/>
-      <c r="V46" s="30"/>
-      <c r="W46" s="30"/>
-      <c r="X46" s="30"/>
-      <c r="Y46" s="30"/>
-      <c r="Z46" s="30"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="31"/>
+      <c r="L46" s="31"/>
+      <c r="M46" s="31"/>
+      <c r="N46" s="31"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="31"/>
+      <c r="S46" s="31"/>
+      <c r="T46" s="31"/>
+      <c r="U46" s="31"/>
+      <c r="V46" s="31"/>
+      <c r="W46" s="31"/>
+      <c r="X46" s="31"/>
+      <c r="Y46" s="31"/>
+      <c r="Z46" s="31"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30" t="s">
-        <v>954</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>955</v>
-      </c>
-      <c r="D47" s="30"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="31" t="s">
+        <v>969</v>
+      </c>
+      <c r="C47" s="31" t="s">
+        <v>970</v>
+      </c>
+      <c r="D47" s="31"/>
       <c r="E47" s="21" t="s">
-        <v>956</v>
-      </c>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
-      <c r="O47" s="30"/>
-      <c r="P47" s="30"/>
-      <c r="Q47" s="30"/>
-      <c r="R47" s="30"/>
-      <c r="S47" s="30"/>
-      <c r="T47" s="30"/>
-      <c r="U47" s="30"/>
-      <c r="V47" s="30"/>
-      <c r="W47" s="30"/>
-      <c r="X47" s="30"/>
-      <c r="Y47" s="30"/>
-      <c r="Z47" s="30"/>
+        <v>971</v>
+      </c>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
+      <c r="N47" s="31"/>
+      <c r="O47" s="31"/>
+      <c r="P47" s="31"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="31"/>
+      <c r="S47" s="31"/>
+      <c r="T47" s="31"/>
+      <c r="U47" s="31"/>
+      <c r="V47" s="31"/>
+      <c r="W47" s="31"/>
+      <c r="X47" s="31"/>
+      <c r="Y47" s="31"/>
+      <c r="Z47" s="31"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
       <c r="E48" s="21" t="s">
-        <v>957</v>
-      </c>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="30"/>
-      <c r="L48" s="30"/>
-      <c r="M48" s="30"/>
-      <c r="N48" s="30"/>
-      <c r="O48" s="30"/>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="30"/>
-      <c r="R48" s="30"/>
-      <c r="S48" s="30"/>
-      <c r="T48" s="30"/>
-      <c r="U48" s="30"/>
-      <c r="V48" s="30"/>
-      <c r="W48" s="30"/>
-      <c r="X48" s="30"/>
-      <c r="Y48" s="30"/>
-      <c r="Z48" s="30"/>
+        <v>972</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
+      <c r="I48" s="31"/>
+      <c r="J48" s="31"/>
+      <c r="K48" s="31"/>
+      <c r="L48" s="31"/>
+      <c r="M48" s="31"/>
+      <c r="N48" s="31"/>
+      <c r="O48" s="31"/>
+      <c r="P48" s="31"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="31"/>
+      <c r="S48" s="31"/>
+      <c r="T48" s="31"/>
+      <c r="U48" s="31"/>
+      <c r="V48" s="31"/>
+      <c r="W48" s="31"/>
+      <c r="X48" s="31"/>
+      <c r="Y48" s="31"/>
+      <c r="Z48" s="31"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="31"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
       <c r="E49" s="21" t="s">
-        <v>958</v>
-      </c>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="30"/>
-      <c r="L49" s="30"/>
-      <c r="M49" s="30"/>
-      <c r="N49" s="30"/>
-      <c r="O49" s="30"/>
-      <c r="P49" s="30"/>
-      <c r="Q49" s="30"/>
-      <c r="R49" s="30"/>
-      <c r="S49" s="30"/>
-      <c r="T49" s="30"/>
-      <c r="U49" s="30"/>
-      <c r="V49" s="30"/>
-      <c r="W49" s="30"/>
-      <c r="X49" s="30"/>
-      <c r="Y49" s="30"/>
-      <c r="Z49" s="30"/>
+        <v>973</v>
+      </c>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
+      <c r="O49" s="31"/>
+      <c r="P49" s="31"/>
+      <c r="Q49" s="31"/>
+      <c r="R49" s="31"/>
+      <c r="S49" s="31"/>
+      <c r="T49" s="31"/>
+      <c r="U49" s="31"/>
+      <c r="V49" s="31"/>
+      <c r="W49" s="31"/>
+      <c r="X49" s="31"/>
+      <c r="Y49" s="31"/>
+      <c r="Z49" s="31"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -15951,22 +16183,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>195</v>
       </c>
     </row>
@@ -15981,7 +16213,7 @@
         <v>236</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>959</v>
+        <v>974</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>237</v>
@@ -16001,7 +16233,7 @@
         <v>273</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>960</v>
+        <v>975</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>210</v>
@@ -16021,7 +16253,7 @@
         <v>285</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>961</v>
+        <v>976</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>237</v>
@@ -16041,7 +16273,7 @@
         <v>448</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>962</v>
+        <v>977</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>306</v>
@@ -16058,7 +16290,7 @@
         <v>529</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>963</v>
+        <v>978</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>306</v>
@@ -16075,7 +16307,7 @@
         <v>416</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>964</v>
+        <v>979</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>306</v>
@@ -16092,7 +16324,7 @@
         <v>420</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>964</v>
+        <v>979</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>306</v>
@@ -16109,7 +16341,7 @@
         <v>429</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>965</v>
+        <v>980</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>306</v>
@@ -16117,16 +16349,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>966</v>
+        <v>981</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>967</v>
+        <v>982</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>968</v>
+        <v>983</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>969</v>
+        <v>984</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>306</v>
@@ -16143,7 +16375,7 @@
         <v>389</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>970</v>
+        <v>985</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>306</v>
@@ -16157,10 +16389,10 @@
         <v>452</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>971</v>
+        <v>986</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>972</v>
+        <v>987</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>306</v>
@@ -16168,16 +16400,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>973</v>
+        <v>988</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>974</v>
+        <v>989</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>975</v>
+        <v>990</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>976</v>
+        <v>991</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>306</v>
@@ -16185,16 +16417,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>977</v>
+        <v>992</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>978</v>
+        <v>993</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>979</v>
+        <v>994</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>980</v>
+        <v>995</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>306</v>
@@ -16208,10 +16440,10 @@
         <v>571</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>981</v>
+        <v>996</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>982</v>
+        <v>997</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>306</v>
@@ -16228,7 +16460,7 @@
         <v>534</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>983</v>
+        <v>998</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>859</v>
@@ -16245,7 +16477,7 @@
         <v>772</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>984</v>
+        <v>999</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>237</v>
@@ -16265,7 +16497,7 @@
         <v>777</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>985</v>
+        <v>1000</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>306</v>
@@ -16350,7 +16582,7 @@
         <v>596</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>986</v>
+        <v>1001</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>237</v>
@@ -16370,7 +16602,7 @@
         <v>523</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>987</v>
+        <v>1002</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>237</v>
@@ -16387,10 +16619,10 @@
         <v>896</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>988</v>
+        <v>1003</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>989</v>
+        <v>1004</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>237</v>
@@ -16410,7 +16642,7 @@
         <v>893</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>990</v>
+        <v>1005</v>
       </c>
       <c r="E26" s="0" t="s">
         <v>306</v>
@@ -16438,16 +16670,16 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>991</v>
+        <v>1006</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>992</v>
+        <v>1007</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>993</v>
+        <v>1008</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>994</v>
+        <v>1009</v>
       </c>
       <c r="E28" s="0" t="s">
         <v>237</v>
@@ -16467,7 +16699,7 @@
         <v>346</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>995</v>
+        <v>1010</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>237</v>
@@ -16487,7 +16719,7 @@
         <v>350</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>996</v>
+        <v>1011</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>306</v>
@@ -16495,16 +16727,16 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>997</v>
+        <v>1012</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>998</v>
+        <v>1013</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>999</v>
+        <v>1014</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>1000</v>
+        <v>1015</v>
       </c>
       <c r="E31" s="0" t="s">
         <v>237</v>
@@ -16524,7 +16756,7 @@
         <v>548</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>1001</v>
+        <v>1016</v>
       </c>
       <c r="E32" s="0" t="s">
         <v>306</v>
@@ -16544,7 +16776,7 @@
         <v>830</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>1002</v>
+        <v>1017</v>
       </c>
       <c r="E33" s="0" t="s">
         <v>237</v>
@@ -16564,7 +16796,7 @@
         <v>834</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>1003</v>
+        <v>1018</v>
       </c>
       <c r="E34" s="0" t="s">
         <v>237</v>
@@ -16608,83 +16840,83 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1004</v>
+        <v>1019</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1005</v>
+        <v>1020</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1006</v>
+        <v>1021</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1007</v>
+        <v>1022</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="34" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1008</v>
+        <v>1023</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1009</v>
+        <v>1024</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1010</v>
+        <v>1025</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1011</v>
+        <v>1026</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="34" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="501.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1012</v>
+        <v>1027</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1013</v>
+        <v>1028</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1014</v>
+        <v>1029</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1015</v>
+        <v>1030</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>1016</v>
+      <c r="F4" s="35" t="s">
+        <v>1031</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16698,7 +16930,7 @@
         <v>497</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>1017</v>
+        <v>1032</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>249</v>
@@ -16709,16 +16941,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1018</v>
+        <v>1033</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>1019</v>
+        <v>1034</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>1020</v>
+        <v>1035</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>1021</v>
+        <v>1036</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>306</v>
@@ -16726,19 +16958,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1022</v>
+        <v>1037</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>1023</v>
+        <v>1038</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>1024</v>
+        <v>1039</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>1025</v>
+        <v>1040</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>1023</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16801,37 +17033,37 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1026</v>
+        <v>1041</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>1027</v>
+        <v>1042</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1028</v>
+        <v>1043</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>1029</v>
+        <v>1044</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>249</v>
@@ -16839,42 +17071,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1030</v>
+        <v>1045</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>1031</v>
+        <v>1046</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1032</v>
+        <v>1047</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1033</v>
+        <v>1048</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="F3" s="35" t="s">
-        <v>1034</v>
+      <c r="F3" s="36" t="s">
+        <v>1049</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1035</v>
+        <v>1050</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>1036</v>
+        <v>1051</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>1037</v>
+        <v>1052</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>1038</v>
+        <v>1053</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="F4" s="35" t="s">
-        <v>1039</v>
+      <c r="F4" s="36" t="s">
+        <v>1054</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
removed terminationDate and priceAtTerminationDate for CEG
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2485" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2483" uniqueCount="1055">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -10421,9 +10421,7 @@
       <c r="S79" s="19" t="s">
         <v>598</v>
       </c>
-      <c r="T79" s="19" t="s">
-        <v>598</v>
-      </c>
+      <c r="T79" s="19"/>
       <c r="U79" s="22"/>
       <c r="V79" s="19" t="s">
         <v>598</v>
@@ -10495,9 +10493,7 @@
       <c r="S80" s="19" t="s">
         <v>603</v>
       </c>
-      <c r="T80" s="19" t="s">
-        <v>603</v>
-      </c>
+      <c r="T80" s="19"/>
       <c r="U80" s="22"/>
       <c r="V80" s="19" t="s">
         <v>603</v>

</xml_diff>

<commit_message>
added intraday day count convention enum options
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -1440,10 +1440,15 @@
 option: 2, identifier: actualThreeSixtyFive, name: Actual Three Sixty Five, acronym: A365, description: Year fractions accrue on the basis of the actual number of days per month and 365 days per year in the respective period.
 option: 3, identifier: thirtyEThreeSixtyISDA, name: Thirty E Three Sixty ISDA, acronym: 30E360ISDA, description: Year fractions accrue on the basis of 30 days per month and 360 days per year in the respective period (ISDA method).
 option: 4, identifier: thirtyEThreeSixty, name: Thirty E Three Sixty, acronym: 30E360, description: Year fractions accrue on the basis of 30 days per month and 360 days per year in the respective period.
-option: 5, identifier: twentyEightEThreeThirtySix, name: Twenty Eight E Three Thirty Six, acronym: 28E336, description: Year fractions accrue on the basis of 28 days per month and 336 days per year in the respective period.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Method defining how days are counted between two dates. This finally defines the year fraction in accrual calculations.</t>
+option: 5, identifier: twentyEightEThreeThirtySix, name: Twenty Eight E Three Thirty Six, acronym: 28E336, description: Year fractions accrue on the basis of 28 days per month and 336 days per year in the respective period.
+option: 6, identifier: one, name: One, acronym: ONE, description: Year fractions are always 1.
+option: 7, identifier: oneByTwelve, name: One by Twelve, acronym: OBYT, description: Year fractions are always 1/12.
+option: 8, identifier: hoursActualActual, name: Hours/Actual/Actual, acronym: HRSAA, description: Year fractions accrue on the basis of measured hours between two timestamps assuming every day counts 24 hours, the actual number of days per month and the actual number of days per year in the respective period.
+option: 9, identifier: minutesActualActual, name: Minutes/Actual/Actual, acronym: MINAA, description: Year fractions accrue on the basis of measured minutes between two timestamps assuming every every day counts 1440 minutes, the actual number of days per month and the actual number of days per year in the respective period.
+option: 10, identifier: secondsActualActual, name: Seconds/Actual/Actual, acronym: SECAA, description: Year fractions accrue on the basis of measured seconds between two timestamps assuming every day counts 86400 seconds, the actual number of days per month and the actual number of days per year in the respective period.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method defining how the time periods between any two timestamps of a full year are measured. This finally defines the year fraction e.g. in interest accrual calculations.</t>
   </si>
   <si>
     <t xml:space="preserve">accruedInterest</t>

</xml_diff>

<commit_message>
fixed formatting error in day count convention term
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -1442,10 +1442,10 @@
 option: 4, identifier: thirtyEThreeSixty, name: Thirty E Three Sixty, acronym: 30E360, description: Year fractions accrue on the basis of 30 days per month and 360 days per year in the respective period.
 option: 5, identifier: twentyEightEThreeThirtySix, name: Twenty Eight E Three Thirty Six, acronym: 28E336, description: Year fractions accrue on the basis of 28 days per month and 336 days per year in the respective period.
 option: 6, identifier: one, name: One, acronym: ONE, description: Year fractions are always 1.
-option: 7, identifier: oneByTwelve, name: One by Twelve, acronym: OBYT, description: Year fractions are always 1/12.
-option: 8, identifier: hoursActualActual, name: Hours/Actual/Actual, acronym: HRSAA, description: Year fractions accrue on the basis of measured hours between two timestamps assuming every day counts 24 hours, the actual number of days per month and the actual number of days per year in the respective period.
-option: 9, identifier: minutesActualActual, name: Minutes/Actual/Actual, acronym: MINAA, description: Year fractions accrue on the basis of measured minutes between two timestamps assuming every every day counts 1440 minutes, the actual number of days per month and the actual number of days per year in the respective period.
-option: 10, identifier: secondsActualActual, name: Seconds/Actual/Actual, acronym: SECAA, description: Year fractions accrue on the basis of measured seconds between two timestamps assuming every day counts 86400 seconds, the actual number of days per month and the actual number of days per year in the respective period.</t>
+option: 7, identifier: oneByTwelve, name: One by Twelve, acronym: OBYT, description: Year fractions are always 1 divided by 12.
+option: 8, identifier: hoursActualActual, name: Hours/Actual/Actual, acronym: HRSAA, description: Year fractions accrue on the basis of measured hours between two timestamps assuming every day counts 24 hours and the actual number of days per month and the actual number of days per year in the respective period.
+option: 9, identifier: minutesActualActual, name: Minutes/Actual/Actual, acronym: MINAA, description: Year fractions accrue on the basis of measured minutes between two timestamps assuming every every day counts 1440 minutes and the actual number of days per month and the actual number of days per year in the respective period.
+option: 10, identifier: secondsActualActual, name: Seconds/Actual/Actual, acronym: SECAA, description: Year fractions accrue on the basis of measured seconds between two timestamps assuming every day counts 86400 seconds and the actual number of days per month and the actual number of days per year in the respective period.</t>
   </si>
   <si>
     <t xml:space="preserve">Method defining how the time periods between any two timestamps of a full year are measured. This finally defines the year fraction e.g. in interest accrual calculations.</t>

</xml_diff>